<commit_message>
adds pathways and networks
</commit_message>
<xml_diff>
--- a/topic_ontologies_glittr.xlsx
+++ b/topic_ontologies_glittr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geertvangeest/Documents/repositories/glittr-ontologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CB3235-13D0-D34B-ABD6-090BB03BC2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D37C07-0642-D744-8C67-715A26578604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="500" windowWidth="28920" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Blad1!$B$1:$G$1016</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Blad1!$B$1:$G$1017</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="183">
   <si>
     <t>Containerization</t>
   </si>
@@ -629,6 +629,18 @@
   </si>
   <si>
     <t>Workflow engine and language. It aims to reduce the complexity of creating workflows by providing a fast and comfortable execution environment, together with a clean and modern domain specific specification language (DSL) in python style.</t>
+  </si>
+  <si>
+    <t>Pathways and Networks</t>
+  </si>
+  <si>
+    <t>Pathway or network</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_2600</t>
+  </si>
+  <si>
+    <t>Primary data about a specific biological pathway or network (the nodes and connections within the pathway or network).</t>
   </si>
 </sst>
 </file>
@@ -812,6 +824,16 @@
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -821,12 +843,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FFA4C2F4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -841,8 +869,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -859,22 +887,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB4A7D6"/>
           <bgColor rgb="FFB4A7D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA4C2F4"/>
-          <bgColor rgb="FFA4C2F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1092,10 +1104,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1016"/>
+  <dimension ref="A1:G1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1833,7 +1845,7 @@
         <v>87</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f t="shared" ref="E34:E54" si="1">IF(D34=B34,"TRUE", "FALSE")</f>
+        <f t="shared" ref="E34:E55" si="1">IF(D34=B34,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -2231,72 +2243,72 @@
       <c r="A51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>136</v>
+      <c r="B51" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FALSE</v>
       </c>
-      <c r="F51" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>139</v>
+      <c r="F51" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>FALSE</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>146</v>
+      <c r="B53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>TRUE</v>
       </c>
-      <c r="F53" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G53" t="s">
-        <v>148</v>
+      <c r="F53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2304,27 +2316,48 @@
         <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
+        <v>TRUE</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>FALSE</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F55" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="14"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="14"/>
@@ -2356,7 +2389,7 @@
     <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="14"/>
     </row>
     <row r="67" spans="1:1" ht="13" x14ac:dyDescent="0.15">
@@ -5209,34 +5242,37 @@
     <row r="1016" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1016" s="14"/>
     </row>
+    <row r="1017" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1017" s="14"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:G1016" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A2:A209">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Statistics and machine learning">
+  <autoFilter ref="B1:G1017" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A2:A210">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Omics analysis">
+      <formula>NOT(ISERROR(SEARCH(("Omics analysis"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Computational methods and pipelines">
+      <formula>NOT(ISERROR(SEARCH(("Computational methods and pipelines"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Statistics and machine learning">
       <formula>NOT(ISERROR(SEARCH(("Statistics and machine learning"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Scripting and languages">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Others">
+      <formula>NOT(ISERROR(SEARCH(("Others"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Scripting and languages">
       <formula>NOT(ISERROR(SEARCH(("Scripting and languages"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Omics analysis">
-      <formula>NOT(ISERROR(SEARCH(("Omics analysis"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Computational methods and pipelines">
-      <formula>NOT(ISERROR(SEARCH(("Computational methods and pipelines"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Reproducibility and data management">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Reproducibility and data management">
       <formula>NOT(ISERROR(SEARCH(("Reproducibility and data management"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Others">
-      <formula>NOT(ISERROR(SEARCH(("Others"),(A2))))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E55">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"TRUE"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E54">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FALSE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -5277,10 +5313,10 @@
     <hyperlink ref="F46" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="F47" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="F48" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F51" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="F52" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F53" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="F54" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F52" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F53" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F54" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F55" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
     <hyperlink ref="F29" r:id="rId42" location="Java" xr:uid="{3A663C11-DD57-8645-8EA4-87B1D3250EC5}"/>
     <hyperlink ref="F30" r:id="rId43" location="C_C++" xr:uid="{C3B74948-F199-1447-B670-8BC72A89A5F8}"/>
     <hyperlink ref="F7" r:id="rId44" xr:uid="{88DBBF94-CB57-854D-88FD-606D4268F8B7}"/>
@@ -5289,8 +5325,9 @@
     <hyperlink ref="F26" r:id="rId47" xr:uid="{B464ED92-6ECB-FA47-B395-204A441448BD}"/>
     <hyperlink ref="F49" r:id="rId48" xr:uid="{A0059E1D-2F4F-F94D-A5C9-290682EE3BF6}"/>
     <hyperlink ref="F50" r:id="rId49" xr:uid="{2A9A0FA4-3276-CA43-BC5E-8130D6536487}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{E0B47E6A-ED88-8441-8475-761ED87B3B20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId50"/>
+  <legacyDrawing r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates tags with wikipedia entry
</commit_message>
<xml_diff>
--- a/topic_ontologies_glittr.xlsx
+++ b/topic_ontologies_glittr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geertvangeest/Documents/repositories/glittr-ontologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D37C07-0642-D744-8C67-715A26578604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67E023B-F07B-264F-B0FE-E99C35348499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="500" windowWidth="28920" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="191">
   <si>
     <t>Containerization</t>
   </si>
@@ -641,13 +641,37 @@
   </si>
   <si>
     <t>Primary data about a specific biological pathway or network (the nodes and connections within the pathway or network).</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Shiny (software)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Shiny_(software)</t>
+  </si>
+  <si>
+    <t>Shiny is a free and open source R package for developing web applications (apps).</t>
+  </si>
+  <si>
+    <t>Julia (programming language)</t>
+  </si>
+  <si>
+    <t>Julia is a high-level, general-purpose dynamic programming language, most commonly used for numerical analysis and computational science.</t>
+  </si>
+  <si>
+    <t>Make (software)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make is a build automation tool that builds executable programs and libraries from source code by reading files called makefiles which specify how to derive the target program. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -739,6 +763,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -803,7 +833,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -816,22 +845,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -843,18 +863,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA4C2F4"/>
-          <bgColor rgb="FFA4C2F4"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -869,8 +883,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -887,6 +901,22 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB4A7D6"/>
           <bgColor rgb="FFB4A7D6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1106,8 +1136,8 @@
   </sheetPr>
   <dimension ref="A1:G1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1258,20 +1288,20 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1300,23 +1330,23 @@
       <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1579,10 +1609,22 @@
       <c r="B22" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="C22" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
+      <c r="F22" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
@@ -1639,13 +1681,21 @@
       <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>187</v>
+      </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>166</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1655,12 +1705,21 @@
       <c r="B26" t="s">
         <v>68</v>
       </c>
+      <c r="C26" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>189</v>
+      </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="14" t="s">
         <v>167</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1715,23 +1774,23 @@
       <c r="A29" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>153</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="15" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1739,23 +1798,23 @@
       <c r="A30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>156</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>156</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="15" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1790,7 +1849,7 @@
       <c r="B32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2112,7 +2171,7 @@
         <f t="shared" si="1"/>
         <v>TRUE</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="12" t="s">
         <v>123</v>
       </c>
       <c r="G45" t="s">
@@ -2126,7 +2185,7 @@
       <c r="B46" t="s">
         <v>126</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D46" t="s">
@@ -2195,23 +2254,23 @@
       <c r="A49" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>168</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="13" t="s">
         <v>168</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>TRUE</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="13" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2219,23 +2278,23 @@
       <c r="A50" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>171</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="13" t="s">
         <v>171</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>TRUE</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="13" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2243,23 +2302,23 @@
       <c r="A51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>179</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="13" t="s">
         <v>180</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FALSE</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="13" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2270,7 +2329,7 @@
       <c r="B52" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -2360,2919 +2419,2919 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="14"/>
+      <c r="A56" s="13"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="14"/>
+      <c r="A57" s="13"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="14"/>
+      <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="14"/>
+      <c r="A59" s="13"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="14"/>
+      <c r="A60" s="13"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="14"/>
+      <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="14"/>
+      <c r="A62" s="13"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="14"/>
+      <c r="A63" s="13"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="14"/>
+      <c r="A64" s="13"/>
     </row>
     <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="14"/>
+      <c r="A65" s="13"/>
     </row>
     <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="14"/>
+      <c r="A66" s="13"/>
     </row>
     <row r="67" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="14"/>
+      <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="14"/>
+      <c r="A68" s="13"/>
     </row>
     <row r="69" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A69" s="14"/>
+      <c r="A69" s="13"/>
     </row>
     <row r="70" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="14"/>
+      <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A71" s="14"/>
+      <c r="A71" s="13"/>
     </row>
     <row r="72" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A72" s="14"/>
+      <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A73" s="14"/>
+      <c r="A73" s="13"/>
     </row>
     <row r="74" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A74" s="14"/>
+      <c r="A74" s="13"/>
     </row>
     <row r="75" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="14"/>
+      <c r="A75" s="13"/>
     </row>
     <row r="76" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="14"/>
+      <c r="A76" s="13"/>
     </row>
     <row r="77" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A77" s="14"/>
+      <c r="A77" s="13"/>
     </row>
     <row r="78" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A78" s="14"/>
+      <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A79" s="14"/>
+      <c r="A79" s="13"/>
     </row>
     <row r="80" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A80" s="14"/>
+      <c r="A80" s="13"/>
     </row>
     <row r="81" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A81" s="14"/>
+      <c r="A81" s="13"/>
     </row>
     <row r="82" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A82" s="14"/>
+      <c r="A82" s="13"/>
     </row>
     <row r="83" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A83" s="14"/>
+      <c r="A83" s="13"/>
     </row>
     <row r="84" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A84" s="14"/>
+      <c r="A84" s="13"/>
     </row>
     <row r="85" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A85" s="14"/>
+      <c r="A85" s="13"/>
     </row>
     <row r="86" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="14"/>
+      <c r="A86" s="13"/>
     </row>
     <row r="87" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="14"/>
+      <c r="A87" s="13"/>
     </row>
     <row r="88" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="14"/>
+      <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A89" s="14"/>
+      <c r="A89" s="13"/>
     </row>
     <row r="90" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="14"/>
+      <c r="A90" s="13"/>
     </row>
     <row r="91" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A91" s="14"/>
+      <c r="A91" s="13"/>
     </row>
     <row r="92" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A92" s="14"/>
+      <c r="A92" s="13"/>
     </row>
     <row r="93" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A93" s="14"/>
+      <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A94" s="14"/>
+      <c r="A94" s="13"/>
     </row>
     <row r="95" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A95" s="14"/>
+      <c r="A95" s="13"/>
     </row>
     <row r="96" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="14"/>
+      <c r="A96" s="13"/>
     </row>
     <row r="97" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A97" s="14"/>
+      <c r="A97" s="13"/>
     </row>
     <row r="98" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A98" s="14"/>
+      <c r="A98" s="13"/>
     </row>
     <row r="99" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A99" s="14"/>
+      <c r="A99" s="13"/>
     </row>
     <row r="100" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A100" s="14"/>
+      <c r="A100" s="13"/>
     </row>
     <row r="101" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A101" s="14"/>
+      <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A102" s="14"/>
+      <c r="A102" s="13"/>
     </row>
     <row r="103" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A103" s="14"/>
+      <c r="A103" s="13"/>
     </row>
     <row r="104" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A104" s="14"/>
+      <c r="A104" s="13"/>
     </row>
     <row r="105" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A105" s="14"/>
+      <c r="A105" s="13"/>
     </row>
     <row r="106" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A106" s="14"/>
+      <c r="A106" s="13"/>
     </row>
     <row r="107" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A107" s="14"/>
+      <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A108" s="14"/>
+      <c r="A108" s="13"/>
     </row>
     <row r="109" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A109" s="14"/>
+      <c r="A109" s="13"/>
     </row>
     <row r="110" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A110" s="14"/>
+      <c r="A110" s="13"/>
     </row>
     <row r="111" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A111" s="14"/>
+      <c r="A111" s="13"/>
     </row>
     <row r="112" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A112" s="14"/>
+      <c r="A112" s="13"/>
     </row>
     <row r="113" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A113" s="14"/>
+      <c r="A113" s="13"/>
     </row>
     <row r="114" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A114" s="14"/>
+      <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A115" s="14"/>
+      <c r="A115" s="13"/>
     </row>
     <row r="116" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A116" s="14"/>
+      <c r="A116" s="13"/>
     </row>
     <row r="117" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A117" s="14"/>
+      <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A118" s="14"/>
+      <c r="A118" s="13"/>
     </row>
     <row r="119" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A119" s="14"/>
+      <c r="A119" s="13"/>
     </row>
     <row r="120" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A120" s="14"/>
+      <c r="A120" s="13"/>
     </row>
     <row r="121" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A121" s="14"/>
+      <c r="A121" s="13"/>
     </row>
     <row r="122" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A122" s="14"/>
+      <c r="A122" s="13"/>
     </row>
     <row r="123" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A123" s="14"/>
+      <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A124" s="14"/>
+      <c r="A124" s="13"/>
     </row>
     <row r="125" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A125" s="14"/>
+      <c r="A125" s="13"/>
     </row>
     <row r="126" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A126" s="14"/>
+      <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A127" s="14"/>
+      <c r="A127" s="13"/>
     </row>
     <row r="128" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A128" s="14"/>
+      <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A129" s="14"/>
+      <c r="A129" s="13"/>
     </row>
     <row r="130" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A130" s="14"/>
+      <c r="A130" s="13"/>
     </row>
     <row r="131" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A131" s="14"/>
+      <c r="A131" s="13"/>
     </row>
     <row r="132" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A132" s="14"/>
+      <c r="A132" s="13"/>
     </row>
     <row r="133" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A133" s="14"/>
+      <c r="A133" s="13"/>
     </row>
     <row r="134" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A134" s="14"/>
+      <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A135" s="14"/>
+      <c r="A135" s="13"/>
     </row>
     <row r="136" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A136" s="14"/>
+      <c r="A136" s="13"/>
     </row>
     <row r="137" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A137" s="14"/>
+      <c r="A137" s="13"/>
     </row>
     <row r="138" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A138" s="14"/>
+      <c r="A138" s="13"/>
     </row>
     <row r="139" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A139" s="14"/>
+      <c r="A139" s="13"/>
     </row>
     <row r="140" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A140" s="14"/>
+      <c r="A140" s="13"/>
     </row>
     <row r="141" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A141" s="14"/>
+      <c r="A141" s="13"/>
     </row>
     <row r="142" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A142" s="14"/>
+      <c r="A142" s="13"/>
     </row>
     <row r="143" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A143" s="14"/>
+      <c r="A143" s="13"/>
     </row>
     <row r="144" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A144" s="14"/>
+      <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A145" s="14"/>
+      <c r="A145" s="13"/>
     </row>
     <row r="146" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A146" s="14"/>
+      <c r="A146" s="13"/>
     </row>
     <row r="147" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A147" s="14"/>
+      <c r="A147" s="13"/>
     </row>
     <row r="148" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A148" s="14"/>
+      <c r="A148" s="13"/>
     </row>
     <row r="149" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A149" s="14"/>
+      <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A150" s="14"/>
+      <c r="A150" s="13"/>
     </row>
     <row r="151" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A151" s="14"/>
+      <c r="A151" s="13"/>
     </row>
     <row r="152" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A152" s="14"/>
+      <c r="A152" s="13"/>
     </row>
     <row r="153" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A153" s="14"/>
+      <c r="A153" s="13"/>
     </row>
     <row r="154" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A154" s="14"/>
+      <c r="A154" s="13"/>
     </row>
     <row r="155" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A155" s="14"/>
+      <c r="A155" s="13"/>
     </row>
     <row r="156" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A156" s="14"/>
+      <c r="A156" s="13"/>
     </row>
     <row r="157" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A157" s="14"/>
+      <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A158" s="14"/>
+      <c r="A158" s="13"/>
     </row>
     <row r="159" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A159" s="14"/>
+      <c r="A159" s="13"/>
     </row>
     <row r="160" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A160" s="14"/>
+      <c r="A160" s="13"/>
     </row>
     <row r="161" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A161" s="14"/>
+      <c r="A161" s="13"/>
     </row>
     <row r="162" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A162" s="14"/>
+      <c r="A162" s="13"/>
     </row>
     <row r="163" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A163" s="14"/>
+      <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A164" s="14"/>
+      <c r="A164" s="13"/>
     </row>
     <row r="165" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A165" s="14"/>
+      <c r="A165" s="13"/>
     </row>
     <row r="166" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A166" s="14"/>
+      <c r="A166" s="13"/>
     </row>
     <row r="167" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A167" s="14"/>
+      <c r="A167" s="13"/>
     </row>
     <row r="168" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A168" s="14"/>
+      <c r="A168" s="13"/>
     </row>
     <row r="169" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A169" s="14"/>
+      <c r="A169" s="13"/>
     </row>
     <row r="170" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A170" s="14"/>
+      <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A171" s="14"/>
+      <c r="A171" s="13"/>
     </row>
     <row r="172" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A172" s="14"/>
+      <c r="A172" s="13"/>
     </row>
     <row r="173" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A173" s="14"/>
+      <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A174" s="14"/>
+      <c r="A174" s="13"/>
     </row>
     <row r="175" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A175" s="14"/>
+      <c r="A175" s="13"/>
     </row>
     <row r="176" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A176" s="14"/>
+      <c r="A176" s="13"/>
     </row>
     <row r="177" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A177" s="14"/>
+      <c r="A177" s="13"/>
     </row>
     <row r="178" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A178" s="14"/>
+      <c r="A178" s="13"/>
     </row>
     <row r="179" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A179" s="14"/>
+      <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A180" s="14"/>
+      <c r="A180" s="13"/>
     </row>
     <row r="181" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A181" s="14"/>
+      <c r="A181" s="13"/>
     </row>
     <row r="182" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A182" s="14"/>
+      <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A183" s="14"/>
+      <c r="A183" s="13"/>
     </row>
     <row r="184" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A184" s="14"/>
+      <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A185" s="14"/>
+      <c r="A185" s="13"/>
     </row>
     <row r="186" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A186" s="14"/>
+      <c r="A186" s="13"/>
     </row>
     <row r="187" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A187" s="14"/>
+      <c r="A187" s="13"/>
     </row>
     <row r="188" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A188" s="14"/>
+      <c r="A188" s="13"/>
     </row>
     <row r="189" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A189" s="14"/>
+      <c r="A189" s="13"/>
     </row>
     <row r="190" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A190" s="14"/>
+      <c r="A190" s="13"/>
     </row>
     <row r="191" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A191" s="14"/>
+      <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A192" s="14"/>
+      <c r="A192" s="13"/>
     </row>
     <row r="193" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A193" s="14"/>
+      <c r="A193" s="13"/>
     </row>
     <row r="194" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A194" s="14"/>
+      <c r="A194" s="13"/>
     </row>
     <row r="195" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A195" s="14"/>
+      <c r="A195" s="13"/>
     </row>
     <row r="196" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A196" s="14"/>
+      <c r="A196" s="13"/>
     </row>
     <row r="197" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A197" s="14"/>
+      <c r="A197" s="13"/>
     </row>
     <row r="198" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A198" s="14"/>
+      <c r="A198" s="13"/>
     </row>
     <row r="199" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A199" s="14"/>
+      <c r="A199" s="13"/>
     </row>
     <row r="200" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A200" s="14"/>
+      <c r="A200" s="13"/>
     </row>
     <row r="201" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A201" s="14"/>
+      <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A202" s="14"/>
+      <c r="A202" s="13"/>
     </row>
     <row r="203" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A203" s="14"/>
+      <c r="A203" s="13"/>
     </row>
     <row r="204" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A204" s="14"/>
+      <c r="A204" s="13"/>
     </row>
     <row r="205" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A205" s="14"/>
+      <c r="A205" s="13"/>
     </row>
     <row r="206" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A206" s="14"/>
+      <c r="A206" s="13"/>
     </row>
     <row r="207" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A207" s="14"/>
+      <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A208" s="14"/>
+      <c r="A208" s="13"/>
     </row>
     <row r="209" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A209" s="14"/>
+      <c r="A209" s="13"/>
     </row>
     <row r="210" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A210" s="14"/>
+      <c r="A210" s="13"/>
     </row>
     <row r="211" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A211" s="14"/>
+      <c r="A211" s="13"/>
     </row>
     <row r="212" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A212" s="14"/>
+      <c r="A212" s="13"/>
     </row>
     <row r="213" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A213" s="14"/>
+      <c r="A213" s="13"/>
     </row>
     <row r="214" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A214" s="14"/>
+      <c r="A214" s="13"/>
     </row>
     <row r="215" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A215" s="14"/>
+      <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A216" s="14"/>
+      <c r="A216" s="13"/>
     </row>
     <row r="217" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A217" s="14"/>
+      <c r="A217" s="13"/>
     </row>
     <row r="218" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A218" s="14"/>
+      <c r="A218" s="13"/>
     </row>
     <row r="219" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A219" s="14"/>
+      <c r="A219" s="13"/>
     </row>
     <row r="220" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A220" s="14"/>
+      <c r="A220" s="13"/>
     </row>
     <row r="221" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A221" s="14"/>
+      <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A222" s="14"/>
+      <c r="A222" s="13"/>
     </row>
     <row r="223" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A223" s="14"/>
+      <c r="A223" s="13"/>
     </row>
     <row r="224" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A224" s="14"/>
+      <c r="A224" s="13"/>
     </row>
     <row r="225" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A225" s="14"/>
+      <c r="A225" s="13"/>
     </row>
     <row r="226" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A226" s="14"/>
+      <c r="A226" s="13"/>
     </row>
     <row r="227" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A227" s="14"/>
+      <c r="A227" s="13"/>
     </row>
     <row r="228" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A228" s="14"/>
+      <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A229" s="14"/>
+      <c r="A229" s="13"/>
     </row>
     <row r="230" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A230" s="14"/>
+      <c r="A230" s="13"/>
     </row>
     <row r="231" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A231" s="14"/>
+      <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A232" s="14"/>
+      <c r="A232" s="13"/>
     </row>
     <row r="233" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A233" s="14"/>
+      <c r="A233" s="13"/>
     </row>
     <row r="234" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A234" s="14"/>
+      <c r="A234" s="13"/>
     </row>
     <row r="235" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A235" s="14"/>
+      <c r="A235" s="13"/>
     </row>
     <row r="236" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A236" s="14"/>
+      <c r="A236" s="13"/>
     </row>
     <row r="237" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A237" s="14"/>
+      <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A238" s="14"/>
+      <c r="A238" s="13"/>
     </row>
     <row r="239" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A239" s="14"/>
+      <c r="A239" s="13"/>
     </row>
     <row r="240" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A240" s="14"/>
+      <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A241" s="14"/>
+      <c r="A241" s="13"/>
     </row>
     <row r="242" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A242" s="14"/>
+      <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A243" s="14"/>
+      <c r="A243" s="13"/>
     </row>
     <row r="244" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A244" s="14"/>
+      <c r="A244" s="13"/>
     </row>
     <row r="245" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A245" s="14"/>
+      <c r="A245" s="13"/>
     </row>
     <row r="246" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A246" s="14"/>
+      <c r="A246" s="13"/>
     </row>
     <row r="247" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A247" s="14"/>
+      <c r="A247" s="13"/>
     </row>
     <row r="248" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A248" s="14"/>
+      <c r="A248" s="13"/>
     </row>
     <row r="249" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A249" s="14"/>
+      <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A250" s="14"/>
+      <c r="A250" s="13"/>
     </row>
     <row r="251" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A251" s="14"/>
+      <c r="A251" s="13"/>
     </row>
     <row r="252" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A252" s="14"/>
+      <c r="A252" s="13"/>
     </row>
     <row r="253" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A253" s="14"/>
+      <c r="A253" s="13"/>
     </row>
     <row r="254" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A254" s="14"/>
+      <c r="A254" s="13"/>
     </row>
     <row r="255" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A255" s="14"/>
+      <c r="A255" s="13"/>
     </row>
     <row r="256" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A256" s="14"/>
+      <c r="A256" s="13"/>
     </row>
     <row r="257" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A257" s="14"/>
+      <c r="A257" s="13"/>
     </row>
     <row r="258" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A258" s="14"/>
+      <c r="A258" s="13"/>
     </row>
     <row r="259" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A259" s="14"/>
+      <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A260" s="14"/>
+      <c r="A260" s="13"/>
     </row>
     <row r="261" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A261" s="14"/>
+      <c r="A261" s="13"/>
     </row>
     <row r="262" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A262" s="14"/>
+      <c r="A262" s="13"/>
     </row>
     <row r="263" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A263" s="14"/>
+      <c r="A263" s="13"/>
     </row>
     <row r="264" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A264" s="14"/>
+      <c r="A264" s="13"/>
     </row>
     <row r="265" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A265" s="14"/>
+      <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A266" s="14"/>
+      <c r="A266" s="13"/>
     </row>
     <row r="267" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A267" s="14"/>
+      <c r="A267" s="13"/>
     </row>
     <row r="268" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A268" s="14"/>
+      <c r="A268" s="13"/>
     </row>
     <row r="269" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A269" s="14"/>
+      <c r="A269" s="13"/>
     </row>
     <row r="270" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A270" s="14"/>
+      <c r="A270" s="13"/>
     </row>
     <row r="271" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A271" s="14"/>
+      <c r="A271" s="13"/>
     </row>
     <row r="272" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A272" s="14"/>
+      <c r="A272" s="13"/>
     </row>
     <row r="273" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A273" s="14"/>
+      <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A274" s="14"/>
+      <c r="A274" s="13"/>
     </row>
     <row r="275" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A275" s="14"/>
+      <c r="A275" s="13"/>
     </row>
     <row r="276" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A276" s="14"/>
+      <c r="A276" s="13"/>
     </row>
     <row r="277" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A277" s="14"/>
+      <c r="A277" s="13"/>
     </row>
     <row r="278" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A278" s="14"/>
+      <c r="A278" s="13"/>
     </row>
     <row r="279" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A279" s="14"/>
+      <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A280" s="14"/>
+      <c r="A280" s="13"/>
     </row>
     <row r="281" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A281" s="14"/>
+      <c r="A281" s="13"/>
     </row>
     <row r="282" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A282" s="14"/>
+      <c r="A282" s="13"/>
     </row>
     <row r="283" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A283" s="14"/>
+      <c r="A283" s="13"/>
     </row>
     <row r="284" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A284" s="14"/>
+      <c r="A284" s="13"/>
     </row>
     <row r="285" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A285" s="14"/>
+      <c r="A285" s="13"/>
     </row>
     <row r="286" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A286" s="14"/>
+      <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A287" s="14"/>
+      <c r="A287" s="13"/>
     </row>
     <row r="288" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A288" s="14"/>
+      <c r="A288" s="13"/>
     </row>
     <row r="289" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A289" s="14"/>
+      <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A290" s="14"/>
+      <c r="A290" s="13"/>
     </row>
     <row r="291" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A291" s="14"/>
+      <c r="A291" s="13"/>
     </row>
     <row r="292" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A292" s="14"/>
+      <c r="A292" s="13"/>
     </row>
     <row r="293" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A293" s="14"/>
+      <c r="A293" s="13"/>
     </row>
     <row r="294" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A294" s="14"/>
+      <c r="A294" s="13"/>
     </row>
     <row r="295" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A295" s="14"/>
+      <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A296" s="14"/>
+      <c r="A296" s="13"/>
     </row>
     <row r="297" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A297" s="14"/>
+      <c r="A297" s="13"/>
     </row>
     <row r="298" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A298" s="14"/>
+      <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A299" s="14"/>
+      <c r="A299" s="13"/>
     </row>
     <row r="300" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A300" s="14"/>
+      <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A301" s="14"/>
+      <c r="A301" s="13"/>
     </row>
     <row r="302" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A302" s="14"/>
+      <c r="A302" s="13"/>
     </row>
     <row r="303" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A303" s="14"/>
+      <c r="A303" s="13"/>
     </row>
     <row r="304" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A304" s="14"/>
+      <c r="A304" s="13"/>
     </row>
     <row r="305" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A305" s="14"/>
+      <c r="A305" s="13"/>
     </row>
     <row r="306" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A306" s="14"/>
+      <c r="A306" s="13"/>
     </row>
     <row r="307" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A307" s="14"/>
+      <c r="A307" s="13"/>
     </row>
     <row r="308" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A308" s="14"/>
+      <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A309" s="14"/>
+      <c r="A309" s="13"/>
     </row>
     <row r="310" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A310" s="14"/>
+      <c r="A310" s="13"/>
     </row>
     <row r="311" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A311" s="14"/>
+      <c r="A311" s="13"/>
     </row>
     <row r="312" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A312" s="14"/>
+      <c r="A312" s="13"/>
     </row>
     <row r="313" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A313" s="14"/>
+      <c r="A313" s="13"/>
     </row>
     <row r="314" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A314" s="14"/>
+      <c r="A314" s="13"/>
     </row>
     <row r="315" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A315" s="14"/>
+      <c r="A315" s="13"/>
     </row>
     <row r="316" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A316" s="14"/>
+      <c r="A316" s="13"/>
     </row>
     <row r="317" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A317" s="14"/>
+      <c r="A317" s="13"/>
     </row>
     <row r="318" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A318" s="14"/>
+      <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A319" s="14"/>
+      <c r="A319" s="13"/>
     </row>
     <row r="320" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A320" s="14"/>
+      <c r="A320" s="13"/>
     </row>
     <row r="321" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A321" s="14"/>
+      <c r="A321" s="13"/>
     </row>
     <row r="322" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A322" s="14"/>
+      <c r="A322" s="13"/>
     </row>
     <row r="323" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A323" s="14"/>
+      <c r="A323" s="13"/>
     </row>
     <row r="324" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A324" s="14"/>
+      <c r="A324" s="13"/>
     </row>
     <row r="325" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A325" s="14"/>
+      <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A326" s="14"/>
+      <c r="A326" s="13"/>
     </row>
     <row r="327" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A327" s="14"/>
+      <c r="A327" s="13"/>
     </row>
     <row r="328" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A328" s="14"/>
+      <c r="A328" s="13"/>
     </row>
     <row r="329" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A329" s="14"/>
+      <c r="A329" s="13"/>
     </row>
     <row r="330" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A330" s="14"/>
+      <c r="A330" s="13"/>
     </row>
     <row r="331" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A331" s="14"/>
+      <c r="A331" s="13"/>
     </row>
     <row r="332" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A332" s="14"/>
+      <c r="A332" s="13"/>
     </row>
     <row r="333" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A333" s="14"/>
+      <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A334" s="14"/>
+      <c r="A334" s="13"/>
     </row>
     <row r="335" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A335" s="14"/>
+      <c r="A335" s="13"/>
     </row>
     <row r="336" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A336" s="14"/>
+      <c r="A336" s="13"/>
     </row>
     <row r="337" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A337" s="14"/>
+      <c r="A337" s="13"/>
     </row>
     <row r="338" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A338" s="14"/>
+      <c r="A338" s="13"/>
     </row>
     <row r="339" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A339" s="14"/>
+      <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A340" s="14"/>
+      <c r="A340" s="13"/>
     </row>
     <row r="341" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A341" s="14"/>
+      <c r="A341" s="13"/>
     </row>
     <row r="342" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A342" s="14"/>
+      <c r="A342" s="13"/>
     </row>
     <row r="343" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A343" s="14"/>
+      <c r="A343" s="13"/>
     </row>
     <row r="344" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A344" s="14"/>
+      <c r="A344" s="13"/>
     </row>
     <row r="345" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A345" s="14"/>
+      <c r="A345" s="13"/>
     </row>
     <row r="346" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A346" s="14"/>
+      <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A347" s="14"/>
+      <c r="A347" s="13"/>
     </row>
     <row r="348" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A348" s="14"/>
+      <c r="A348" s="13"/>
     </row>
     <row r="349" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A349" s="14"/>
+      <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A350" s="14"/>
+      <c r="A350" s="13"/>
     </row>
     <row r="351" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A351" s="14"/>
+      <c r="A351" s="13"/>
     </row>
     <row r="352" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A352" s="14"/>
+      <c r="A352" s="13"/>
     </row>
     <row r="353" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A353" s="14"/>
+      <c r="A353" s="13"/>
     </row>
     <row r="354" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A354" s="14"/>
+      <c r="A354" s="13"/>
     </row>
     <row r="355" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A355" s="14"/>
+      <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A356" s="14"/>
+      <c r="A356" s="13"/>
     </row>
     <row r="357" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A357" s="14"/>
+      <c r="A357" s="13"/>
     </row>
     <row r="358" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A358" s="14"/>
+      <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A359" s="14"/>
+      <c r="A359" s="13"/>
     </row>
     <row r="360" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A360" s="14"/>
+      <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A361" s="14"/>
+      <c r="A361" s="13"/>
     </row>
     <row r="362" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A362" s="14"/>
+      <c r="A362" s="13"/>
     </row>
     <row r="363" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A363" s="14"/>
+      <c r="A363" s="13"/>
     </row>
     <row r="364" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A364" s="14"/>
+      <c r="A364" s="13"/>
     </row>
     <row r="365" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A365" s="14"/>
+      <c r="A365" s="13"/>
     </row>
     <row r="366" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A366" s="14"/>
+      <c r="A366" s="13"/>
     </row>
     <row r="367" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A367" s="14"/>
+      <c r="A367" s="13"/>
     </row>
     <row r="368" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A368" s="14"/>
+      <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A369" s="14"/>
+      <c r="A369" s="13"/>
     </row>
     <row r="370" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A370" s="14"/>
+      <c r="A370" s="13"/>
     </row>
     <row r="371" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A371" s="14"/>
+      <c r="A371" s="13"/>
     </row>
     <row r="372" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A372" s="14"/>
+      <c r="A372" s="13"/>
     </row>
     <row r="373" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A373" s="14"/>
+      <c r="A373" s="13"/>
     </row>
     <row r="374" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A374" s="14"/>
+      <c r="A374" s="13"/>
     </row>
     <row r="375" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A375" s="14"/>
+      <c r="A375" s="13"/>
     </row>
     <row r="376" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A376" s="14"/>
+      <c r="A376" s="13"/>
     </row>
     <row r="377" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A377" s="14"/>
+      <c r="A377" s="13"/>
     </row>
     <row r="378" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A378" s="14"/>
+      <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A379" s="14"/>
+      <c r="A379" s="13"/>
     </row>
     <row r="380" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A380" s="14"/>
+      <c r="A380" s="13"/>
     </row>
     <row r="381" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A381" s="14"/>
+      <c r="A381" s="13"/>
     </row>
     <row r="382" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A382" s="14"/>
+      <c r="A382" s="13"/>
     </row>
     <row r="383" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A383" s="14"/>
+      <c r="A383" s="13"/>
     </row>
     <row r="384" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A384" s="14"/>
+      <c r="A384" s="13"/>
     </row>
     <row r="385" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A385" s="14"/>
+      <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A386" s="14"/>
+      <c r="A386" s="13"/>
     </row>
     <row r="387" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A387" s="14"/>
+      <c r="A387" s="13"/>
     </row>
     <row r="388" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A388" s="14"/>
+      <c r="A388" s="13"/>
     </row>
     <row r="389" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A389" s="14"/>
+      <c r="A389" s="13"/>
     </row>
     <row r="390" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A390" s="14"/>
+      <c r="A390" s="13"/>
     </row>
     <row r="391" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A391" s="14"/>
+      <c r="A391" s="13"/>
     </row>
     <row r="392" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A392" s="14"/>
+      <c r="A392" s="13"/>
     </row>
     <row r="393" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A393" s="14"/>
+      <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A394" s="14"/>
+      <c r="A394" s="13"/>
     </row>
     <row r="395" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A395" s="14"/>
+      <c r="A395" s="13"/>
     </row>
     <row r="396" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A396" s="14"/>
+      <c r="A396" s="13"/>
     </row>
     <row r="397" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A397" s="14"/>
+      <c r="A397" s="13"/>
     </row>
     <row r="398" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A398" s="14"/>
+      <c r="A398" s="13"/>
     </row>
     <row r="399" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A399" s="14"/>
+      <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A400" s="14"/>
+      <c r="A400" s="13"/>
     </row>
     <row r="401" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A401" s="14"/>
+      <c r="A401" s="13"/>
     </row>
     <row r="402" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A402" s="14"/>
+      <c r="A402" s="13"/>
     </row>
     <row r="403" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A403" s="14"/>
+      <c r="A403" s="13"/>
     </row>
     <row r="404" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A404" s="14"/>
+      <c r="A404" s="13"/>
     </row>
     <row r="405" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A405" s="14"/>
+      <c r="A405" s="13"/>
     </row>
     <row r="406" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A406" s="14"/>
+      <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A407" s="14"/>
+      <c r="A407" s="13"/>
     </row>
     <row r="408" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A408" s="14"/>
+      <c r="A408" s="13"/>
     </row>
     <row r="409" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A409" s="14"/>
+      <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A410" s="14"/>
+      <c r="A410" s="13"/>
     </row>
     <row r="411" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A411" s="14"/>
+      <c r="A411" s="13"/>
     </row>
     <row r="412" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A412" s="14"/>
+      <c r="A412" s="13"/>
     </row>
     <row r="413" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A413" s="14"/>
+      <c r="A413" s="13"/>
     </row>
     <row r="414" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A414" s="14"/>
+      <c r="A414" s="13"/>
     </row>
     <row r="415" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A415" s="14"/>
+      <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A416" s="14"/>
+      <c r="A416" s="13"/>
     </row>
     <row r="417" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A417" s="14"/>
+      <c r="A417" s="13"/>
     </row>
     <row r="418" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A418" s="14"/>
+      <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A419" s="14"/>
+      <c r="A419" s="13"/>
     </row>
     <row r="420" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A420" s="14"/>
+      <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A421" s="14"/>
+      <c r="A421" s="13"/>
     </row>
     <row r="422" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A422" s="14"/>
+      <c r="A422" s="13"/>
     </row>
     <row r="423" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A423" s="14"/>
+      <c r="A423" s="13"/>
     </row>
     <row r="424" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A424" s="14"/>
+      <c r="A424" s="13"/>
     </row>
     <row r="425" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A425" s="14"/>
+      <c r="A425" s="13"/>
     </row>
     <row r="426" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A426" s="14"/>
+      <c r="A426" s="13"/>
     </row>
     <row r="427" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A427" s="14"/>
+      <c r="A427" s="13"/>
     </row>
     <row r="428" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A428" s="14"/>
+      <c r="A428" s="13"/>
     </row>
     <row r="429" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A429" s="14"/>
+      <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A430" s="14"/>
+      <c r="A430" s="13"/>
     </row>
     <row r="431" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A431" s="14"/>
+      <c r="A431" s="13"/>
     </row>
     <row r="432" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A432" s="14"/>
+      <c r="A432" s="13"/>
     </row>
     <row r="433" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A433" s="14"/>
+      <c r="A433" s="13"/>
     </row>
     <row r="434" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A434" s="14"/>
+      <c r="A434" s="13"/>
     </row>
     <row r="435" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A435" s="14"/>
+      <c r="A435" s="13"/>
     </row>
     <row r="436" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A436" s="14"/>
+      <c r="A436" s="13"/>
     </row>
     <row r="437" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A437" s="14"/>
+      <c r="A437" s="13"/>
     </row>
     <row r="438" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A438" s="14"/>
+      <c r="A438" s="13"/>
     </row>
     <row r="439" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A439" s="14"/>
+      <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A440" s="14"/>
+      <c r="A440" s="13"/>
     </row>
     <row r="441" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A441" s="14"/>
+      <c r="A441" s="13"/>
     </row>
     <row r="442" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A442" s="14"/>
+      <c r="A442" s="13"/>
     </row>
     <row r="443" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A443" s="14"/>
+      <c r="A443" s="13"/>
     </row>
     <row r="444" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A444" s="14"/>
+      <c r="A444" s="13"/>
     </row>
     <row r="445" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A445" s="14"/>
+      <c r="A445" s="13"/>
     </row>
     <row r="446" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A446" s="14"/>
+      <c r="A446" s="13"/>
     </row>
     <row r="447" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A447" s="14"/>
+      <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A448" s="14"/>
+      <c r="A448" s="13"/>
     </row>
     <row r="449" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A449" s="14"/>
+      <c r="A449" s="13"/>
     </row>
     <row r="450" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A450" s="14"/>
+      <c r="A450" s="13"/>
     </row>
     <row r="451" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A451" s="14"/>
+      <c r="A451" s="13"/>
     </row>
     <row r="452" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A452" s="14"/>
+      <c r="A452" s="13"/>
     </row>
     <row r="453" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A453" s="14"/>
+      <c r="A453" s="13"/>
     </row>
     <row r="454" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A454" s="14"/>
+      <c r="A454" s="13"/>
     </row>
     <row r="455" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A455" s="14"/>
+      <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A456" s="14"/>
+      <c r="A456" s="13"/>
     </row>
     <row r="457" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A457" s="14"/>
+      <c r="A457" s="13"/>
     </row>
     <row r="458" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A458" s="14"/>
+      <c r="A458" s="13"/>
     </row>
     <row r="459" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A459" s="14"/>
+      <c r="A459" s="13"/>
     </row>
     <row r="460" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A460" s="14"/>
+      <c r="A460" s="13"/>
     </row>
     <row r="461" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A461" s="14"/>
+      <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A462" s="14"/>
+      <c r="A462" s="13"/>
     </row>
     <row r="463" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A463" s="14"/>
+      <c r="A463" s="13"/>
     </row>
     <row r="464" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A464" s="14"/>
+      <c r="A464" s="13"/>
     </row>
     <row r="465" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A465" s="14"/>
+      <c r="A465" s="13"/>
     </row>
     <row r="466" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A466" s="14"/>
+      <c r="A466" s="13"/>
     </row>
     <row r="467" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A467" s="14"/>
+      <c r="A467" s="13"/>
     </row>
     <row r="468" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A468" s="14"/>
+      <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A469" s="14"/>
+      <c r="A469" s="13"/>
     </row>
     <row r="470" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A470" s="14"/>
+      <c r="A470" s="13"/>
     </row>
     <row r="471" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A471" s="14"/>
+      <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A472" s="14"/>
+      <c r="A472" s="13"/>
     </row>
     <row r="473" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A473" s="14"/>
+      <c r="A473" s="13"/>
     </row>
     <row r="474" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A474" s="14"/>
+      <c r="A474" s="13"/>
     </row>
     <row r="475" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A475" s="14"/>
+      <c r="A475" s="13"/>
     </row>
     <row r="476" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A476" s="14"/>
+      <c r="A476" s="13"/>
     </row>
     <row r="477" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A477" s="14"/>
+      <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A478" s="14"/>
+      <c r="A478" s="13"/>
     </row>
     <row r="479" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A479" s="14"/>
+      <c r="A479" s="13"/>
     </row>
     <row r="480" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A480" s="14"/>
+      <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A481" s="14"/>
+      <c r="A481" s="13"/>
     </row>
     <row r="482" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A482" s="14"/>
+      <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A483" s="14"/>
+      <c r="A483" s="13"/>
     </row>
     <row r="484" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A484" s="14"/>
+      <c r="A484" s="13"/>
     </row>
     <row r="485" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A485" s="14"/>
+      <c r="A485" s="13"/>
     </row>
     <row r="486" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A486" s="14"/>
+      <c r="A486" s="13"/>
     </row>
     <row r="487" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A487" s="14"/>
+      <c r="A487" s="13"/>
     </row>
     <row r="488" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A488" s="14"/>
+      <c r="A488" s="13"/>
     </row>
     <row r="489" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A489" s="14"/>
+      <c r="A489" s="13"/>
     </row>
     <row r="490" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A490" s="14"/>
+      <c r="A490" s="13"/>
     </row>
     <row r="491" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A491" s="14"/>
+      <c r="A491" s="13"/>
     </row>
     <row r="492" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A492" s="14"/>
+      <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A493" s="14"/>
+      <c r="A493" s="13"/>
     </row>
     <row r="494" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A494" s="14"/>
+      <c r="A494" s="13"/>
     </row>
     <row r="495" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A495" s="14"/>
+      <c r="A495" s="13"/>
     </row>
     <row r="496" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A496" s="14"/>
+      <c r="A496" s="13"/>
     </row>
     <row r="497" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A497" s="14"/>
+      <c r="A497" s="13"/>
     </row>
     <row r="498" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A498" s="14"/>
+      <c r="A498" s="13"/>
     </row>
     <row r="499" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A499" s="14"/>
+      <c r="A499" s="13"/>
     </row>
     <row r="500" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A500" s="14"/>
+      <c r="A500" s="13"/>
     </row>
     <row r="501" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A501" s="14"/>
+      <c r="A501" s="13"/>
     </row>
     <row r="502" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A502" s="14"/>
+      <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A503" s="14"/>
+      <c r="A503" s="13"/>
     </row>
     <row r="504" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A504" s="14"/>
+      <c r="A504" s="13"/>
     </row>
     <row r="505" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A505" s="14"/>
+      <c r="A505" s="13"/>
     </row>
     <row r="506" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A506" s="14"/>
+      <c r="A506" s="13"/>
     </row>
     <row r="507" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A507" s="14"/>
+      <c r="A507" s="13"/>
     </row>
     <row r="508" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A508" s="14"/>
+      <c r="A508" s="13"/>
     </row>
     <row r="509" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A509" s="14"/>
+      <c r="A509" s="13"/>
     </row>
     <row r="510" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A510" s="14"/>
+      <c r="A510" s="13"/>
     </row>
     <row r="511" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A511" s="14"/>
+      <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A512" s="14"/>
+      <c r="A512" s="13"/>
     </row>
     <row r="513" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A513" s="14"/>
+      <c r="A513" s="13"/>
     </row>
     <row r="514" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A514" s="14"/>
+      <c r="A514" s="13"/>
     </row>
     <row r="515" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A515" s="14"/>
+      <c r="A515" s="13"/>
     </row>
     <row r="516" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A516" s="14"/>
+      <c r="A516" s="13"/>
     </row>
     <row r="517" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A517" s="14"/>
+      <c r="A517" s="13"/>
     </row>
     <row r="518" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A518" s="14"/>
+      <c r="A518" s="13"/>
     </row>
     <row r="519" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A519" s="14"/>
+      <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A520" s="14"/>
+      <c r="A520" s="13"/>
     </row>
     <row r="521" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A521" s="14"/>
+      <c r="A521" s="13"/>
     </row>
     <row r="522" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A522" s="14"/>
+      <c r="A522" s="13"/>
     </row>
     <row r="523" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A523" s="14"/>
+      <c r="A523" s="13"/>
     </row>
     <row r="524" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A524" s="14"/>
+      <c r="A524" s="13"/>
     </row>
     <row r="525" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A525" s="14"/>
+      <c r="A525" s="13"/>
     </row>
     <row r="526" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A526" s="14"/>
+      <c r="A526" s="13"/>
     </row>
     <row r="527" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A527" s="14"/>
+      <c r="A527" s="13"/>
     </row>
     <row r="528" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A528" s="14"/>
+      <c r="A528" s="13"/>
     </row>
     <row r="529" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A529" s="14"/>
+      <c r="A529" s="13"/>
     </row>
     <row r="530" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A530" s="14"/>
+      <c r="A530" s="13"/>
     </row>
     <row r="531" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A531" s="14"/>
+      <c r="A531" s="13"/>
     </row>
     <row r="532" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A532" s="14"/>
+      <c r="A532" s="13"/>
     </row>
     <row r="533" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A533" s="14"/>
+      <c r="A533" s="13"/>
     </row>
     <row r="534" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A534" s="14"/>
+      <c r="A534" s="13"/>
     </row>
     <row r="535" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A535" s="14"/>
+      <c r="A535" s="13"/>
     </row>
     <row r="536" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A536" s="14"/>
+      <c r="A536" s="13"/>
     </row>
     <row r="537" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A537" s="14"/>
+      <c r="A537" s="13"/>
     </row>
     <row r="538" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A538" s="14"/>
+      <c r="A538" s="13"/>
     </row>
     <row r="539" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A539" s="14"/>
+      <c r="A539" s="13"/>
     </row>
     <row r="540" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A540" s="14"/>
+      <c r="A540" s="13"/>
     </row>
     <row r="541" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A541" s="14"/>
+      <c r="A541" s="13"/>
     </row>
     <row r="542" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A542" s="14"/>
+      <c r="A542" s="13"/>
     </row>
     <row r="543" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A543" s="14"/>
+      <c r="A543" s="13"/>
     </row>
     <row r="544" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A544" s="14"/>
+      <c r="A544" s="13"/>
     </row>
     <row r="545" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A545" s="14"/>
+      <c r="A545" s="13"/>
     </row>
     <row r="546" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A546" s="14"/>
+      <c r="A546" s="13"/>
     </row>
     <row r="547" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A547" s="14"/>
+      <c r="A547" s="13"/>
     </row>
     <row r="548" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A548" s="14"/>
+      <c r="A548" s="13"/>
     </row>
     <row r="549" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A549" s="14"/>
+      <c r="A549" s="13"/>
     </row>
     <row r="550" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A550" s="14"/>
+      <c r="A550" s="13"/>
     </row>
     <row r="551" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A551" s="14"/>
+      <c r="A551" s="13"/>
     </row>
     <row r="552" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A552" s="14"/>
+      <c r="A552" s="13"/>
     </row>
     <row r="553" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A553" s="14"/>
+      <c r="A553" s="13"/>
     </row>
     <row r="554" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A554" s="14"/>
+      <c r="A554" s="13"/>
     </row>
     <row r="555" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A555" s="14"/>
+      <c r="A555" s="13"/>
     </row>
     <row r="556" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A556" s="14"/>
+      <c r="A556" s="13"/>
     </row>
     <row r="557" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A557" s="14"/>
+      <c r="A557" s="13"/>
     </row>
     <row r="558" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A558" s="14"/>
+      <c r="A558" s="13"/>
     </row>
     <row r="559" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A559" s="14"/>
+      <c r="A559" s="13"/>
     </row>
     <row r="560" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A560" s="14"/>
+      <c r="A560" s="13"/>
     </row>
     <row r="561" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A561" s="14"/>
+      <c r="A561" s="13"/>
     </row>
     <row r="562" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A562" s="14"/>
+      <c r="A562" s="13"/>
     </row>
     <row r="563" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A563" s="14"/>
+      <c r="A563" s="13"/>
     </row>
     <row r="564" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A564" s="14"/>
+      <c r="A564" s="13"/>
     </row>
     <row r="565" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A565" s="14"/>
+      <c r="A565" s="13"/>
     </row>
     <row r="566" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A566" s="14"/>
+      <c r="A566" s="13"/>
     </row>
     <row r="567" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A567" s="14"/>
+      <c r="A567" s="13"/>
     </row>
     <row r="568" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A568" s="14"/>
+      <c r="A568" s="13"/>
     </row>
     <row r="569" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A569" s="14"/>
+      <c r="A569" s="13"/>
     </row>
     <row r="570" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A570" s="14"/>
+      <c r="A570" s="13"/>
     </row>
     <row r="571" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A571" s="14"/>
+      <c r="A571" s="13"/>
     </row>
     <row r="572" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A572" s="14"/>
+      <c r="A572" s="13"/>
     </row>
     <row r="573" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A573" s="14"/>
+      <c r="A573" s="13"/>
     </row>
     <row r="574" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A574" s="14"/>
+      <c r="A574" s="13"/>
     </row>
     <row r="575" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A575" s="14"/>
+      <c r="A575" s="13"/>
     </row>
     <row r="576" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A576" s="14"/>
+      <c r="A576" s="13"/>
     </row>
     <row r="577" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A577" s="14"/>
+      <c r="A577" s="13"/>
     </row>
     <row r="578" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A578" s="14"/>
+      <c r="A578" s="13"/>
     </row>
     <row r="579" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A579" s="14"/>
+      <c r="A579" s="13"/>
     </row>
     <row r="580" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A580" s="14"/>
+      <c r="A580" s="13"/>
     </row>
     <row r="581" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A581" s="14"/>
+      <c r="A581" s="13"/>
     </row>
     <row r="582" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A582" s="14"/>
+      <c r="A582" s="13"/>
     </row>
     <row r="583" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A583" s="14"/>
+      <c r="A583" s="13"/>
     </row>
     <row r="584" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A584" s="14"/>
+      <c r="A584" s="13"/>
     </row>
     <row r="585" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A585" s="14"/>
+      <c r="A585" s="13"/>
     </row>
     <row r="586" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A586" s="14"/>
+      <c r="A586" s="13"/>
     </row>
     <row r="587" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A587" s="14"/>
+      <c r="A587" s="13"/>
     </row>
     <row r="588" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A588" s="14"/>
+      <c r="A588" s="13"/>
     </row>
     <row r="589" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A589" s="14"/>
+      <c r="A589" s="13"/>
     </row>
     <row r="590" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A590" s="14"/>
+      <c r="A590" s="13"/>
     </row>
     <row r="591" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A591" s="14"/>
+      <c r="A591" s="13"/>
     </row>
     <row r="592" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A592" s="14"/>
+      <c r="A592" s="13"/>
     </row>
     <row r="593" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A593" s="14"/>
+      <c r="A593" s="13"/>
     </row>
     <row r="594" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A594" s="14"/>
+      <c r="A594" s="13"/>
     </row>
     <row r="595" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A595" s="14"/>
+      <c r="A595" s="13"/>
     </row>
     <row r="596" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A596" s="14"/>
+      <c r="A596" s="13"/>
     </row>
     <row r="597" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A597" s="14"/>
+      <c r="A597" s="13"/>
     </row>
     <row r="598" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A598" s="14"/>
+      <c r="A598" s="13"/>
     </row>
     <row r="599" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A599" s="14"/>
+      <c r="A599" s="13"/>
     </row>
     <row r="600" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A600" s="14"/>
+      <c r="A600" s="13"/>
     </row>
     <row r="601" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A601" s="14"/>
+      <c r="A601" s="13"/>
     </row>
     <row r="602" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A602" s="14"/>
+      <c r="A602" s="13"/>
     </row>
     <row r="603" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A603" s="14"/>
+      <c r="A603" s="13"/>
     </row>
     <row r="604" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A604" s="14"/>
+      <c r="A604" s="13"/>
     </row>
     <row r="605" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A605" s="14"/>
+      <c r="A605" s="13"/>
     </row>
     <row r="606" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A606" s="14"/>
+      <c r="A606" s="13"/>
     </row>
     <row r="607" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A607" s="14"/>
+      <c r="A607" s="13"/>
     </row>
     <row r="608" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A608" s="14"/>
+      <c r="A608" s="13"/>
     </row>
     <row r="609" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A609" s="14"/>
+      <c r="A609" s="13"/>
     </row>
     <row r="610" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A610" s="14"/>
+      <c r="A610" s="13"/>
     </row>
     <row r="611" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A611" s="14"/>
+      <c r="A611" s="13"/>
     </row>
     <row r="612" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A612" s="14"/>
+      <c r="A612" s="13"/>
     </row>
     <row r="613" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A613" s="14"/>
+      <c r="A613" s="13"/>
     </row>
     <row r="614" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A614" s="14"/>
+      <c r="A614" s="13"/>
     </row>
     <row r="615" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A615" s="14"/>
+      <c r="A615" s="13"/>
     </row>
     <row r="616" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A616" s="14"/>
+      <c r="A616" s="13"/>
     </row>
     <row r="617" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A617" s="14"/>
+      <c r="A617" s="13"/>
     </row>
     <row r="618" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A618" s="14"/>
+      <c r="A618" s="13"/>
     </row>
     <row r="619" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A619" s="14"/>
+      <c r="A619" s="13"/>
     </row>
     <row r="620" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A620" s="14"/>
+      <c r="A620" s="13"/>
     </row>
     <row r="621" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A621" s="14"/>
+      <c r="A621" s="13"/>
     </row>
     <row r="622" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A622" s="14"/>
+      <c r="A622" s="13"/>
     </row>
     <row r="623" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A623" s="14"/>
+      <c r="A623" s="13"/>
     </row>
     <row r="624" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A624" s="14"/>
+      <c r="A624" s="13"/>
     </row>
     <row r="625" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A625" s="14"/>
+      <c r="A625" s="13"/>
     </row>
     <row r="626" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A626" s="14"/>
+      <c r="A626" s="13"/>
     </row>
     <row r="627" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A627" s="14"/>
+      <c r="A627" s="13"/>
     </row>
     <row r="628" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A628" s="14"/>
+      <c r="A628" s="13"/>
     </row>
     <row r="629" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A629" s="14"/>
+      <c r="A629" s="13"/>
     </row>
     <row r="630" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A630" s="14"/>
+      <c r="A630" s="13"/>
     </row>
     <row r="631" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A631" s="14"/>
+      <c r="A631" s="13"/>
     </row>
     <row r="632" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A632" s="14"/>
+      <c r="A632" s="13"/>
     </row>
     <row r="633" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A633" s="14"/>
+      <c r="A633" s="13"/>
     </row>
     <row r="634" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A634" s="14"/>
+      <c r="A634" s="13"/>
     </row>
     <row r="635" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A635" s="14"/>
+      <c r="A635" s="13"/>
     </row>
     <row r="636" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A636" s="14"/>
+      <c r="A636" s="13"/>
     </row>
     <row r="637" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A637" s="14"/>
+      <c r="A637" s="13"/>
     </row>
     <row r="638" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A638" s="14"/>
+      <c r="A638" s="13"/>
     </row>
     <row r="639" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A639" s="14"/>
+      <c r="A639" s="13"/>
     </row>
     <row r="640" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A640" s="14"/>
+      <c r="A640" s="13"/>
     </row>
     <row r="641" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A641" s="14"/>
+      <c r="A641" s="13"/>
     </row>
     <row r="642" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A642" s="14"/>
+      <c r="A642" s="13"/>
     </row>
     <row r="643" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A643" s="14"/>
+      <c r="A643" s="13"/>
     </row>
     <row r="644" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A644" s="14"/>
+      <c r="A644" s="13"/>
     </row>
     <row r="645" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A645" s="14"/>
+      <c r="A645" s="13"/>
     </row>
     <row r="646" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A646" s="14"/>
+      <c r="A646" s="13"/>
     </row>
     <row r="647" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A647" s="14"/>
+      <c r="A647" s="13"/>
     </row>
     <row r="648" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A648" s="14"/>
+      <c r="A648" s="13"/>
     </row>
     <row r="649" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A649" s="14"/>
+      <c r="A649" s="13"/>
     </row>
     <row r="650" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A650" s="14"/>
+      <c r="A650" s="13"/>
     </row>
     <row r="651" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A651" s="14"/>
+      <c r="A651" s="13"/>
     </row>
     <row r="652" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A652" s="14"/>
+      <c r="A652" s="13"/>
     </row>
     <row r="653" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A653" s="14"/>
+      <c r="A653" s="13"/>
     </row>
     <row r="654" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A654" s="14"/>
+      <c r="A654" s="13"/>
     </row>
     <row r="655" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A655" s="14"/>
+      <c r="A655" s="13"/>
     </row>
     <row r="656" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A656" s="14"/>
+      <c r="A656" s="13"/>
     </row>
     <row r="657" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A657" s="14"/>
+      <c r="A657" s="13"/>
     </row>
     <row r="658" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A658" s="14"/>
+      <c r="A658" s="13"/>
     </row>
     <row r="659" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A659" s="14"/>
+      <c r="A659" s="13"/>
     </row>
     <row r="660" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A660" s="14"/>
+      <c r="A660" s="13"/>
     </row>
     <row r="661" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A661" s="14"/>
+      <c r="A661" s="13"/>
     </row>
     <row r="662" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A662" s="14"/>
+      <c r="A662" s="13"/>
     </row>
     <row r="663" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A663" s="14"/>
+      <c r="A663" s="13"/>
     </row>
     <row r="664" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A664" s="14"/>
+      <c r="A664" s="13"/>
     </row>
     <row r="665" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A665" s="14"/>
+      <c r="A665" s="13"/>
     </row>
     <row r="666" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A666" s="14"/>
+      <c r="A666" s="13"/>
     </row>
     <row r="667" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A667" s="14"/>
+      <c r="A667" s="13"/>
     </row>
     <row r="668" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A668" s="14"/>
+      <c r="A668" s="13"/>
     </row>
     <row r="669" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A669" s="14"/>
+      <c r="A669" s="13"/>
     </row>
     <row r="670" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A670" s="14"/>
+      <c r="A670" s="13"/>
     </row>
     <row r="671" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A671" s="14"/>
+      <c r="A671" s="13"/>
     </row>
     <row r="672" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A672" s="14"/>
+      <c r="A672" s="13"/>
     </row>
     <row r="673" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A673" s="14"/>
+      <c r="A673" s="13"/>
     </row>
     <row r="674" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A674" s="14"/>
+      <c r="A674" s="13"/>
     </row>
     <row r="675" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A675" s="14"/>
+      <c r="A675" s="13"/>
     </row>
     <row r="676" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A676" s="14"/>
+      <c r="A676" s="13"/>
     </row>
     <row r="677" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A677" s="14"/>
+      <c r="A677" s="13"/>
     </row>
     <row r="678" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A678" s="14"/>
+      <c r="A678" s="13"/>
     </row>
     <row r="679" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A679" s="14"/>
+      <c r="A679" s="13"/>
     </row>
     <row r="680" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A680" s="14"/>
+      <c r="A680" s="13"/>
     </row>
     <row r="681" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A681" s="14"/>
+      <c r="A681" s="13"/>
     </row>
     <row r="682" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A682" s="14"/>
+      <c r="A682" s="13"/>
     </row>
     <row r="683" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A683" s="14"/>
+      <c r="A683" s="13"/>
     </row>
     <row r="684" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A684" s="14"/>
+      <c r="A684" s="13"/>
     </row>
     <row r="685" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A685" s="14"/>
+      <c r="A685" s="13"/>
     </row>
     <row r="686" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A686" s="14"/>
+      <c r="A686" s="13"/>
     </row>
     <row r="687" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A687" s="14"/>
+      <c r="A687" s="13"/>
     </row>
     <row r="688" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A688" s="14"/>
+      <c r="A688" s="13"/>
     </row>
     <row r="689" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A689" s="14"/>
+      <c r="A689" s="13"/>
     </row>
     <row r="690" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A690" s="14"/>
+      <c r="A690" s="13"/>
     </row>
     <row r="691" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A691" s="14"/>
+      <c r="A691" s="13"/>
     </row>
     <row r="692" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A692" s="14"/>
+      <c r="A692" s="13"/>
     </row>
     <row r="693" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A693" s="14"/>
+      <c r="A693" s="13"/>
     </row>
     <row r="694" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A694" s="14"/>
+      <c r="A694" s="13"/>
     </row>
     <row r="695" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A695" s="14"/>
+      <c r="A695" s="13"/>
     </row>
     <row r="696" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A696" s="14"/>
+      <c r="A696" s="13"/>
     </row>
     <row r="697" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A697" s="14"/>
+      <c r="A697" s="13"/>
     </row>
     <row r="698" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A698" s="14"/>
+      <c r="A698" s="13"/>
     </row>
     <row r="699" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A699" s="14"/>
+      <c r="A699" s="13"/>
     </row>
     <row r="700" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A700" s="14"/>
+      <c r="A700" s="13"/>
     </row>
     <row r="701" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A701" s="14"/>
+      <c r="A701" s="13"/>
     </row>
     <row r="702" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A702" s="14"/>
+      <c r="A702" s="13"/>
     </row>
     <row r="703" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A703" s="14"/>
+      <c r="A703" s="13"/>
     </row>
     <row r="704" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A704" s="14"/>
+      <c r="A704" s="13"/>
     </row>
     <row r="705" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A705" s="14"/>
+      <c r="A705" s="13"/>
     </row>
     <row r="706" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A706" s="14"/>
+      <c r="A706" s="13"/>
     </row>
     <row r="707" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A707" s="14"/>
+      <c r="A707" s="13"/>
     </row>
     <row r="708" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A708" s="14"/>
+      <c r="A708" s="13"/>
     </row>
     <row r="709" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A709" s="14"/>
+      <c r="A709" s="13"/>
     </row>
     <row r="710" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A710" s="14"/>
+      <c r="A710" s="13"/>
     </row>
     <row r="711" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A711" s="14"/>
+      <c r="A711" s="13"/>
     </row>
     <row r="712" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A712" s="14"/>
+      <c r="A712" s="13"/>
     </row>
     <row r="713" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A713" s="14"/>
+      <c r="A713" s="13"/>
     </row>
     <row r="714" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A714" s="14"/>
+      <c r="A714" s="13"/>
     </row>
     <row r="715" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A715" s="14"/>
+      <c r="A715" s="13"/>
     </row>
     <row r="716" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A716" s="14"/>
+      <c r="A716" s="13"/>
     </row>
     <row r="717" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A717" s="14"/>
+      <c r="A717" s="13"/>
     </row>
     <row r="718" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A718" s="14"/>
+      <c r="A718" s="13"/>
     </row>
     <row r="719" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A719" s="14"/>
+      <c r="A719" s="13"/>
     </row>
     <row r="720" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A720" s="14"/>
+      <c r="A720" s="13"/>
     </row>
     <row r="721" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A721" s="14"/>
+      <c r="A721" s="13"/>
     </row>
     <row r="722" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A722" s="14"/>
+      <c r="A722" s="13"/>
     </row>
     <row r="723" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A723" s="14"/>
+      <c r="A723" s="13"/>
     </row>
     <row r="724" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A724" s="14"/>
+      <c r="A724" s="13"/>
     </row>
     <row r="725" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A725" s="14"/>
+      <c r="A725" s="13"/>
     </row>
     <row r="726" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A726" s="14"/>
+      <c r="A726" s="13"/>
     </row>
     <row r="727" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A727" s="14"/>
+      <c r="A727" s="13"/>
     </row>
     <row r="728" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A728" s="14"/>
+      <c r="A728" s="13"/>
     </row>
     <row r="729" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A729" s="14"/>
+      <c r="A729" s="13"/>
     </row>
     <row r="730" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A730" s="14"/>
+      <c r="A730" s="13"/>
     </row>
     <row r="731" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A731" s="14"/>
+      <c r="A731" s="13"/>
     </row>
     <row r="732" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A732" s="14"/>
+      <c r="A732" s="13"/>
     </row>
     <row r="733" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A733" s="14"/>
+      <c r="A733" s="13"/>
     </row>
     <row r="734" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A734" s="14"/>
+      <c r="A734" s="13"/>
     </row>
     <row r="735" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A735" s="14"/>
+      <c r="A735" s="13"/>
     </row>
     <row r="736" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A736" s="14"/>
+      <c r="A736" s="13"/>
     </row>
     <row r="737" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A737" s="14"/>
+      <c r="A737" s="13"/>
     </row>
     <row r="738" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A738" s="14"/>
+      <c r="A738" s="13"/>
     </row>
     <row r="739" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A739" s="14"/>
+      <c r="A739" s="13"/>
     </row>
     <row r="740" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A740" s="14"/>
+      <c r="A740" s="13"/>
     </row>
     <row r="741" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A741" s="14"/>
+      <c r="A741" s="13"/>
     </row>
     <row r="742" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A742" s="14"/>
+      <c r="A742" s="13"/>
     </row>
     <row r="743" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A743" s="14"/>
+      <c r="A743" s="13"/>
     </row>
     <row r="744" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A744" s="14"/>
+      <c r="A744" s="13"/>
     </row>
     <row r="745" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A745" s="14"/>
+      <c r="A745" s="13"/>
     </row>
     <row r="746" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A746" s="14"/>
+      <c r="A746" s="13"/>
     </row>
     <row r="747" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A747" s="14"/>
+      <c r="A747" s="13"/>
     </row>
     <row r="748" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A748" s="14"/>
+      <c r="A748" s="13"/>
     </row>
     <row r="749" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A749" s="14"/>
+      <c r="A749" s="13"/>
     </row>
     <row r="750" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A750" s="14"/>
+      <c r="A750" s="13"/>
     </row>
     <row r="751" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A751" s="14"/>
+      <c r="A751" s="13"/>
     </row>
     <row r="752" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A752" s="14"/>
+      <c r="A752" s="13"/>
     </row>
     <row r="753" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A753" s="14"/>
+      <c r="A753" s="13"/>
     </row>
     <row r="754" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A754" s="14"/>
+      <c r="A754" s="13"/>
     </row>
     <row r="755" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A755" s="14"/>
+      <c r="A755" s="13"/>
     </row>
     <row r="756" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A756" s="14"/>
+      <c r="A756" s="13"/>
     </row>
     <row r="757" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A757" s="14"/>
+      <c r="A757" s="13"/>
     </row>
     <row r="758" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A758" s="14"/>
+      <c r="A758" s="13"/>
     </row>
     <row r="759" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A759" s="14"/>
+      <c r="A759" s="13"/>
     </row>
     <row r="760" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A760" s="14"/>
+      <c r="A760" s="13"/>
     </row>
     <row r="761" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A761" s="14"/>
+      <c r="A761" s="13"/>
     </row>
     <row r="762" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A762" s="14"/>
+      <c r="A762" s="13"/>
     </row>
     <row r="763" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A763" s="14"/>
+      <c r="A763" s="13"/>
     </row>
     <row r="764" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A764" s="14"/>
+      <c r="A764" s="13"/>
     </row>
     <row r="765" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A765" s="14"/>
+      <c r="A765" s="13"/>
     </row>
     <row r="766" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A766" s="14"/>
+      <c r="A766" s="13"/>
     </row>
     <row r="767" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A767" s="14"/>
+      <c r="A767" s="13"/>
     </row>
     <row r="768" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A768" s="14"/>
+      <c r="A768" s="13"/>
     </row>
     <row r="769" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A769" s="14"/>
+      <c r="A769" s="13"/>
     </row>
     <row r="770" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A770" s="14"/>
+      <c r="A770" s="13"/>
     </row>
     <row r="771" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A771" s="14"/>
+      <c r="A771" s="13"/>
     </row>
     <row r="772" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A772" s="14"/>
+      <c r="A772" s="13"/>
     </row>
     <row r="773" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A773" s="14"/>
+      <c r="A773" s="13"/>
     </row>
     <row r="774" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A774" s="14"/>
+      <c r="A774" s="13"/>
     </row>
     <row r="775" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A775" s="14"/>
+      <c r="A775" s="13"/>
     </row>
     <row r="776" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A776" s="14"/>
+      <c r="A776" s="13"/>
     </row>
     <row r="777" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A777" s="14"/>
+      <c r="A777" s="13"/>
     </row>
     <row r="778" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A778" s="14"/>
+      <c r="A778" s="13"/>
     </row>
     <row r="779" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A779" s="14"/>
+      <c r="A779" s="13"/>
     </row>
     <row r="780" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A780" s="14"/>
+      <c r="A780" s="13"/>
     </row>
     <row r="781" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A781" s="14"/>
+      <c r="A781" s="13"/>
     </row>
     <row r="782" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A782" s="14"/>
+      <c r="A782" s="13"/>
     </row>
     <row r="783" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A783" s="14"/>
+      <c r="A783" s="13"/>
     </row>
     <row r="784" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A784" s="14"/>
+      <c r="A784" s="13"/>
     </row>
     <row r="785" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A785" s="14"/>
+      <c r="A785" s="13"/>
     </row>
     <row r="786" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A786" s="14"/>
+      <c r="A786" s="13"/>
     </row>
     <row r="787" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A787" s="14"/>
+      <c r="A787" s="13"/>
     </row>
     <row r="788" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A788" s="14"/>
+      <c r="A788" s="13"/>
     </row>
     <row r="789" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A789" s="14"/>
+      <c r="A789" s="13"/>
     </row>
     <row r="790" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A790" s="14"/>
+      <c r="A790" s="13"/>
     </row>
     <row r="791" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A791" s="14"/>
+      <c r="A791" s="13"/>
     </row>
     <row r="792" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A792" s="14"/>
+      <c r="A792" s="13"/>
     </row>
     <row r="793" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A793" s="14"/>
+      <c r="A793" s="13"/>
     </row>
     <row r="794" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A794" s="14"/>
+      <c r="A794" s="13"/>
     </row>
     <row r="795" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A795" s="14"/>
+      <c r="A795" s="13"/>
     </row>
     <row r="796" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A796" s="14"/>
+      <c r="A796" s="13"/>
     </row>
     <row r="797" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A797" s="14"/>
+      <c r="A797" s="13"/>
     </row>
     <row r="798" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A798" s="14"/>
+      <c r="A798" s="13"/>
     </row>
     <row r="799" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A799" s="14"/>
+      <c r="A799" s="13"/>
     </row>
     <row r="800" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A800" s="14"/>
+      <c r="A800" s="13"/>
     </row>
     <row r="801" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A801" s="14"/>
+      <c r="A801" s="13"/>
     </row>
     <row r="802" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A802" s="14"/>
+      <c r="A802" s="13"/>
     </row>
     <row r="803" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A803" s="14"/>
+      <c r="A803" s="13"/>
     </row>
     <row r="804" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A804" s="14"/>
+      <c r="A804" s="13"/>
     </row>
     <row r="805" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A805" s="14"/>
+      <c r="A805" s="13"/>
     </row>
     <row r="806" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A806" s="14"/>
+      <c r="A806" s="13"/>
     </row>
     <row r="807" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A807" s="14"/>
+      <c r="A807" s="13"/>
     </row>
     <row r="808" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A808" s="14"/>
+      <c r="A808" s="13"/>
     </row>
     <row r="809" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A809" s="14"/>
+      <c r="A809" s="13"/>
     </row>
     <row r="810" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A810" s="14"/>
+      <c r="A810" s="13"/>
     </row>
     <row r="811" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A811" s="14"/>
+      <c r="A811" s="13"/>
     </row>
     <row r="812" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A812" s="14"/>
+      <c r="A812" s="13"/>
     </row>
     <row r="813" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A813" s="14"/>
+      <c r="A813" s="13"/>
     </row>
     <row r="814" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A814" s="14"/>
+      <c r="A814" s="13"/>
     </row>
     <row r="815" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A815" s="14"/>
+      <c r="A815" s="13"/>
     </row>
     <row r="816" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A816" s="14"/>
+      <c r="A816" s="13"/>
     </row>
     <row r="817" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A817" s="14"/>
+      <c r="A817" s="13"/>
     </row>
     <row r="818" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A818" s="14"/>
+      <c r="A818" s="13"/>
     </row>
     <row r="819" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A819" s="14"/>
+      <c r="A819" s="13"/>
     </row>
     <row r="820" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A820" s="14"/>
+      <c r="A820" s="13"/>
     </row>
     <row r="821" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A821" s="14"/>
+      <c r="A821" s="13"/>
     </row>
     <row r="822" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A822" s="14"/>
+      <c r="A822" s="13"/>
     </row>
     <row r="823" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A823" s="14"/>
+      <c r="A823" s="13"/>
     </row>
     <row r="824" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A824" s="14"/>
+      <c r="A824" s="13"/>
     </row>
     <row r="825" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A825" s="14"/>
+      <c r="A825" s="13"/>
     </row>
     <row r="826" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A826" s="14"/>
+      <c r="A826" s="13"/>
     </row>
     <row r="827" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A827" s="14"/>
+      <c r="A827" s="13"/>
     </row>
     <row r="828" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A828" s="14"/>
+      <c r="A828" s="13"/>
     </row>
     <row r="829" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A829" s="14"/>
+      <c r="A829" s="13"/>
     </row>
     <row r="830" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A830" s="14"/>
+      <c r="A830" s="13"/>
     </row>
     <row r="831" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A831" s="14"/>
+      <c r="A831" s="13"/>
     </row>
     <row r="832" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A832" s="14"/>
+      <c r="A832" s="13"/>
     </row>
     <row r="833" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A833" s="14"/>
+      <c r="A833" s="13"/>
     </row>
     <row r="834" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A834" s="14"/>
+      <c r="A834" s="13"/>
     </row>
     <row r="835" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A835" s="14"/>
+      <c r="A835" s="13"/>
     </row>
     <row r="836" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A836" s="14"/>
+      <c r="A836" s="13"/>
     </row>
     <row r="837" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A837" s="14"/>
+      <c r="A837" s="13"/>
     </row>
     <row r="838" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A838" s="14"/>
+      <c r="A838" s="13"/>
     </row>
     <row r="839" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A839" s="14"/>
+      <c r="A839" s="13"/>
     </row>
     <row r="840" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A840" s="14"/>
+      <c r="A840" s="13"/>
     </row>
     <row r="841" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A841" s="14"/>
+      <c r="A841" s="13"/>
     </row>
     <row r="842" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A842" s="14"/>
+      <c r="A842" s="13"/>
     </row>
     <row r="843" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A843" s="14"/>
+      <c r="A843" s="13"/>
     </row>
     <row r="844" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A844" s="14"/>
+      <c r="A844" s="13"/>
     </row>
     <row r="845" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A845" s="14"/>
+      <c r="A845" s="13"/>
     </row>
     <row r="846" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A846" s="14"/>
+      <c r="A846" s="13"/>
     </row>
     <row r="847" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A847" s="14"/>
+      <c r="A847" s="13"/>
     </row>
     <row r="848" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A848" s="14"/>
+      <c r="A848" s="13"/>
     </row>
     <row r="849" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A849" s="14"/>
+      <c r="A849" s="13"/>
     </row>
     <row r="850" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A850" s="14"/>
+      <c r="A850" s="13"/>
     </row>
     <row r="851" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A851" s="14"/>
+      <c r="A851" s="13"/>
     </row>
     <row r="852" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A852" s="14"/>
+      <c r="A852" s="13"/>
     </row>
     <row r="853" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A853" s="14"/>
+      <c r="A853" s="13"/>
     </row>
     <row r="854" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A854" s="14"/>
+      <c r="A854" s="13"/>
     </row>
     <row r="855" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A855" s="14"/>
+      <c r="A855" s="13"/>
     </row>
     <row r="856" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A856" s="14"/>
+      <c r="A856" s="13"/>
     </row>
     <row r="857" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A857" s="14"/>
+      <c r="A857" s="13"/>
     </row>
     <row r="858" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A858" s="14"/>
+      <c r="A858" s="13"/>
     </row>
     <row r="859" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A859" s="14"/>
+      <c r="A859" s="13"/>
     </row>
     <row r="860" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A860" s="14"/>
+      <c r="A860" s="13"/>
     </row>
     <row r="861" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A861" s="14"/>
+      <c r="A861" s="13"/>
     </row>
     <row r="862" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A862" s="14"/>
+      <c r="A862" s="13"/>
     </row>
     <row r="863" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A863" s="14"/>
+      <c r="A863" s="13"/>
     </row>
     <row r="864" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A864" s="14"/>
+      <c r="A864" s="13"/>
     </row>
     <row r="865" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A865" s="14"/>
+      <c r="A865" s="13"/>
     </row>
     <row r="866" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A866" s="14"/>
+      <c r="A866" s="13"/>
     </row>
     <row r="867" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A867" s="14"/>
+      <c r="A867" s="13"/>
     </row>
     <row r="868" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A868" s="14"/>
+      <c r="A868" s="13"/>
     </row>
     <row r="869" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A869" s="14"/>
+      <c r="A869" s="13"/>
     </row>
     <row r="870" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A870" s="14"/>
+      <c r="A870" s="13"/>
     </row>
     <row r="871" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A871" s="14"/>
+      <c r="A871" s="13"/>
     </row>
     <row r="872" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A872" s="14"/>
+      <c r="A872" s="13"/>
     </row>
     <row r="873" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A873" s="14"/>
+      <c r="A873" s="13"/>
     </row>
     <row r="874" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A874" s="14"/>
+      <c r="A874" s="13"/>
     </row>
     <row r="875" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A875" s="14"/>
+      <c r="A875" s="13"/>
     </row>
     <row r="876" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A876" s="14"/>
+      <c r="A876" s="13"/>
     </row>
     <row r="877" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A877" s="14"/>
+      <c r="A877" s="13"/>
     </row>
     <row r="878" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A878" s="14"/>
+      <c r="A878" s="13"/>
     </row>
     <row r="879" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A879" s="14"/>
+      <c r="A879" s="13"/>
     </row>
     <row r="880" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A880" s="14"/>
+      <c r="A880" s="13"/>
     </row>
     <row r="881" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A881" s="14"/>
+      <c r="A881" s="13"/>
     </row>
     <row r="882" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A882" s="14"/>
+      <c r="A882" s="13"/>
     </row>
     <row r="883" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A883" s="14"/>
+      <c r="A883" s="13"/>
     </row>
     <row r="884" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A884" s="14"/>
+      <c r="A884" s="13"/>
     </row>
     <row r="885" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A885" s="14"/>
+      <c r="A885" s="13"/>
     </row>
     <row r="886" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A886" s="14"/>
+      <c r="A886" s="13"/>
     </row>
     <row r="887" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A887" s="14"/>
+      <c r="A887" s="13"/>
     </row>
     <row r="888" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A888" s="14"/>
+      <c r="A888" s="13"/>
     </row>
     <row r="889" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A889" s="14"/>
+      <c r="A889" s="13"/>
     </row>
     <row r="890" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A890" s="14"/>
+      <c r="A890" s="13"/>
     </row>
     <row r="891" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A891" s="14"/>
+      <c r="A891" s="13"/>
     </row>
     <row r="892" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A892" s="14"/>
+      <c r="A892" s="13"/>
     </row>
     <row r="893" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A893" s="14"/>
+      <c r="A893" s="13"/>
     </row>
     <row r="894" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A894" s="14"/>
+      <c r="A894" s="13"/>
     </row>
     <row r="895" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A895" s="14"/>
+      <c r="A895" s="13"/>
     </row>
     <row r="896" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A896" s="14"/>
+      <c r="A896" s="13"/>
     </row>
     <row r="897" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A897" s="14"/>
+      <c r="A897" s="13"/>
     </row>
     <row r="898" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A898" s="14"/>
+      <c r="A898" s="13"/>
     </row>
     <row r="899" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A899" s="14"/>
+      <c r="A899" s="13"/>
     </row>
     <row r="900" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A900" s="14"/>
+      <c r="A900" s="13"/>
     </row>
     <row r="901" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A901" s="14"/>
+      <c r="A901" s="13"/>
     </row>
     <row r="902" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A902" s="14"/>
+      <c r="A902" s="13"/>
     </row>
     <row r="903" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A903" s="14"/>
+      <c r="A903" s="13"/>
     </row>
     <row r="904" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A904" s="14"/>
+      <c r="A904" s="13"/>
     </row>
     <row r="905" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A905" s="14"/>
+      <c r="A905" s="13"/>
     </row>
     <row r="906" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A906" s="14"/>
+      <c r="A906" s="13"/>
     </row>
     <row r="907" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A907" s="14"/>
+      <c r="A907" s="13"/>
     </row>
     <row r="908" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A908" s="14"/>
+      <c r="A908" s="13"/>
     </row>
     <row r="909" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A909" s="14"/>
+      <c r="A909" s="13"/>
     </row>
     <row r="910" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A910" s="14"/>
+      <c r="A910" s="13"/>
     </row>
     <row r="911" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A911" s="14"/>
+      <c r="A911" s="13"/>
     </row>
     <row r="912" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A912" s="14"/>
+      <c r="A912" s="13"/>
     </row>
     <row r="913" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A913" s="14"/>
+      <c r="A913" s="13"/>
     </row>
     <row r="914" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A914" s="14"/>
+      <c r="A914" s="13"/>
     </row>
     <row r="915" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A915" s="14"/>
+      <c r="A915" s="13"/>
     </row>
     <row r="916" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A916" s="14"/>
+      <c r="A916" s="13"/>
     </row>
     <row r="917" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A917" s="14"/>
+      <c r="A917" s="13"/>
     </row>
     <row r="918" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A918" s="14"/>
+      <c r="A918" s="13"/>
     </row>
     <row r="919" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A919" s="14"/>
+      <c r="A919" s="13"/>
     </row>
     <row r="920" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A920" s="14"/>
+      <c r="A920" s="13"/>
     </row>
     <row r="921" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A921" s="14"/>
+      <c r="A921" s="13"/>
     </row>
     <row r="922" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A922" s="14"/>
+      <c r="A922" s="13"/>
     </row>
     <row r="923" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A923" s="14"/>
+      <c r="A923" s="13"/>
     </row>
     <row r="924" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A924" s="14"/>
+      <c r="A924" s="13"/>
     </row>
     <row r="925" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A925" s="14"/>
+      <c r="A925" s="13"/>
     </row>
     <row r="926" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A926" s="14"/>
+      <c r="A926" s="13"/>
     </row>
     <row r="927" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A927" s="14"/>
+      <c r="A927" s="13"/>
     </row>
     <row r="928" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A928" s="14"/>
+      <c r="A928" s="13"/>
     </row>
     <row r="929" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A929" s="14"/>
+      <c r="A929" s="13"/>
     </row>
     <row r="930" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A930" s="14"/>
+      <c r="A930" s="13"/>
     </row>
     <row r="931" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A931" s="14"/>
+      <c r="A931" s="13"/>
     </row>
     <row r="932" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A932" s="14"/>
+      <c r="A932" s="13"/>
     </row>
     <row r="933" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A933" s="14"/>
+      <c r="A933" s="13"/>
     </row>
     <row r="934" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A934" s="14"/>
+      <c r="A934" s="13"/>
     </row>
     <row r="935" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A935" s="14"/>
+      <c r="A935" s="13"/>
     </row>
     <row r="936" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A936" s="14"/>
+      <c r="A936" s="13"/>
     </row>
     <row r="937" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A937" s="14"/>
+      <c r="A937" s="13"/>
     </row>
     <row r="938" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A938" s="14"/>
+      <c r="A938" s="13"/>
     </row>
     <row r="939" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A939" s="14"/>
+      <c r="A939" s="13"/>
     </row>
     <row r="940" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A940" s="14"/>
+      <c r="A940" s="13"/>
     </row>
     <row r="941" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A941" s="14"/>
+      <c r="A941" s="13"/>
     </row>
     <row r="942" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A942" s="14"/>
+      <c r="A942" s="13"/>
     </row>
     <row r="943" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A943" s="14"/>
+      <c r="A943" s="13"/>
     </row>
     <row r="944" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A944" s="14"/>
+      <c r="A944" s="13"/>
     </row>
     <row r="945" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A945" s="14"/>
+      <c r="A945" s="13"/>
     </row>
     <row r="946" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A946" s="14"/>
+      <c r="A946" s="13"/>
     </row>
     <row r="947" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A947" s="14"/>
+      <c r="A947" s="13"/>
     </row>
     <row r="948" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A948" s="14"/>
+      <c r="A948" s="13"/>
     </row>
     <row r="949" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A949" s="14"/>
+      <c r="A949" s="13"/>
     </row>
     <row r="950" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A950" s="14"/>
+      <c r="A950" s="13"/>
     </row>
     <row r="951" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A951" s="14"/>
+      <c r="A951" s="13"/>
     </row>
     <row r="952" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A952" s="14"/>
+      <c r="A952" s="13"/>
     </row>
     <row r="953" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A953" s="14"/>
+      <c r="A953" s="13"/>
     </row>
     <row r="954" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A954" s="14"/>
+      <c r="A954" s="13"/>
     </row>
     <row r="955" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A955" s="14"/>
+      <c r="A955" s="13"/>
     </row>
     <row r="956" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A956" s="14"/>
+      <c r="A956" s="13"/>
     </row>
     <row r="957" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A957" s="14"/>
+      <c r="A957" s="13"/>
     </row>
     <row r="958" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A958" s="14"/>
+      <c r="A958" s="13"/>
     </row>
     <row r="959" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A959" s="14"/>
+      <c r="A959" s="13"/>
     </row>
     <row r="960" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A960" s="14"/>
+      <c r="A960" s="13"/>
     </row>
     <row r="961" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A961" s="14"/>
+      <c r="A961" s="13"/>
     </row>
     <row r="962" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A962" s="14"/>
+      <c r="A962" s="13"/>
     </row>
     <row r="963" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A963" s="14"/>
+      <c r="A963" s="13"/>
     </row>
     <row r="964" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A964" s="14"/>
+      <c r="A964" s="13"/>
     </row>
     <row r="965" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A965" s="14"/>
+      <c r="A965" s="13"/>
     </row>
     <row r="966" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A966" s="14"/>
+      <c r="A966" s="13"/>
     </row>
     <row r="967" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A967" s="14"/>
+      <c r="A967" s="13"/>
     </row>
     <row r="968" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A968" s="14"/>
+      <c r="A968" s="13"/>
     </row>
     <row r="969" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A969" s="14"/>
+      <c r="A969" s="13"/>
     </row>
     <row r="970" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A970" s="14"/>
+      <c r="A970" s="13"/>
     </row>
     <row r="971" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A971" s="14"/>
+      <c r="A971" s="13"/>
     </row>
     <row r="972" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A972" s="14"/>
+      <c r="A972" s="13"/>
     </row>
     <row r="973" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A973" s="14"/>
+      <c r="A973" s="13"/>
     </row>
     <row r="974" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A974" s="14"/>
+      <c r="A974" s="13"/>
     </row>
     <row r="975" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A975" s="14"/>
+      <c r="A975" s="13"/>
     </row>
     <row r="976" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A976" s="14"/>
+      <c r="A976" s="13"/>
     </row>
     <row r="977" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A977" s="14"/>
+      <c r="A977" s="13"/>
     </row>
     <row r="978" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A978" s="14"/>
+      <c r="A978" s="13"/>
     </row>
     <row r="979" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A979" s="14"/>
+      <c r="A979" s="13"/>
     </row>
     <row r="980" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A980" s="14"/>
+      <c r="A980" s="13"/>
     </row>
     <row r="981" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A981" s="14"/>
+      <c r="A981" s="13"/>
     </row>
     <row r="982" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A982" s="14"/>
+      <c r="A982" s="13"/>
     </row>
     <row r="983" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A983" s="14"/>
+      <c r="A983" s="13"/>
     </row>
     <row r="984" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A984" s="14"/>
+      <c r="A984" s="13"/>
     </row>
     <row r="985" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A985" s="14"/>
+      <c r="A985" s="13"/>
     </row>
     <row r="986" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A986" s="14"/>
+      <c r="A986" s="13"/>
     </row>
     <row r="987" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A987" s="14"/>
+      <c r="A987" s="13"/>
     </row>
     <row r="988" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A988" s="14"/>
+      <c r="A988" s="13"/>
     </row>
     <row r="989" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A989" s="14"/>
+      <c r="A989" s="13"/>
     </row>
     <row r="990" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A990" s="14"/>
+      <c r="A990" s="13"/>
     </row>
     <row r="991" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A991" s="14"/>
+      <c r="A991" s="13"/>
     </row>
     <row r="992" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A992" s="14"/>
+      <c r="A992" s="13"/>
     </row>
     <row r="993" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A993" s="14"/>
+      <c r="A993" s="13"/>
     </row>
     <row r="994" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A994" s="14"/>
+      <c r="A994" s="13"/>
     </row>
     <row r="995" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A995" s="14"/>
+      <c r="A995" s="13"/>
     </row>
     <row r="996" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A996" s="14"/>
+      <c r="A996" s="13"/>
     </row>
     <row r="997" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A997" s="14"/>
+      <c r="A997" s="13"/>
     </row>
     <row r="998" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A998" s="14"/>
+      <c r="A998" s="13"/>
     </row>
     <row r="999" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A999" s="14"/>
+      <c r="A999" s="13"/>
     </row>
     <row r="1000" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1000" s="14"/>
+      <c r="A1000" s="13"/>
     </row>
     <row r="1001" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1001" s="14"/>
+      <c r="A1001" s="13"/>
     </row>
     <row r="1002" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1002" s="14"/>
+      <c r="A1002" s="13"/>
     </row>
     <row r="1003" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1003" s="14"/>
+      <c r="A1003" s="13"/>
     </row>
     <row r="1004" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1004" s="14"/>
+      <c r="A1004" s="13"/>
     </row>
     <row r="1005" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1005" s="14"/>
+      <c r="A1005" s="13"/>
     </row>
     <row r="1006" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1006" s="14"/>
+      <c r="A1006" s="13"/>
     </row>
     <row r="1007" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1007" s="14"/>
+      <c r="A1007" s="13"/>
     </row>
     <row r="1008" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1008" s="14"/>
+      <c r="A1008" s="13"/>
     </row>
     <row r="1009" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1009" s="14"/>
+      <c r="A1009" s="13"/>
     </row>
     <row r="1010" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1010" s="14"/>
+      <c r="A1010" s="13"/>
     </row>
     <row r="1011" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1011" s="14"/>
+      <c r="A1011" s="13"/>
     </row>
     <row r="1012" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1012" s="14"/>
+      <c r="A1012" s="13"/>
     </row>
     <row r="1013" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1013" s="14"/>
+      <c r="A1013" s="13"/>
     </row>
     <row r="1014" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1014" s="14"/>
+      <c r="A1014" s="13"/>
     </row>
     <row r="1015" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1015" s="14"/>
+      <c r="A1015" s="13"/>
     </row>
     <row r="1016" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1016" s="14"/>
+      <c r="A1016" s="13"/>
     </row>
     <row r="1017" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1017" s="14"/>
+      <c r="A1017" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G1017" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A2:A210">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Omics analysis">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Statistics and machine learning">
+      <formula>NOT(ISERROR(SEARCH(("Statistics and machine learning"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Scripting and languages">
+      <formula>NOT(ISERROR(SEARCH(("Scripting and languages"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Omics analysis">
       <formula>NOT(ISERROR(SEARCH(("Omics analysis"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Computational methods and pipelines">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Computational methods and pipelines">
       <formula>NOT(ISERROR(SEARCH(("Computational methods and pipelines"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Statistics and machine learning">
-      <formula>NOT(ISERROR(SEARCH(("Statistics and machine learning"),(A2))))</formula>
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Reproducibility and data management">
+      <formula>NOT(ISERROR(SEARCH(("Reproducibility and data management"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Others">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Others">
       <formula>NOT(ISERROR(SEARCH(("Others"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Scripting and languages">
-      <formula>NOT(ISERROR(SEARCH(("Scripting and languages"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Reproducibility and data management">
-      <formula>NOT(ISERROR(SEARCH(("Reproducibility and data management"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E55">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"FALSE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TRUE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"FALSE"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -5326,8 +5385,9 @@
     <hyperlink ref="F49" r:id="rId48" xr:uid="{A0059E1D-2F4F-F94D-A5C9-290682EE3BF6}"/>
     <hyperlink ref="F50" r:id="rId49" xr:uid="{2A9A0FA4-3276-CA43-BC5E-8130D6536487}"/>
     <hyperlink ref="F51" r:id="rId50" xr:uid="{E0B47E6A-ED88-8441-8475-761ED87B3B20}"/>
+    <hyperlink ref="F22" r:id="rId51" xr:uid="{C3FF2065-443C-594B-A3F7-7A818E41D753}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId51"/>
+  <legacyDrawing r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adds term_code and term_set to excel sheet
</commit_message>
<xml_diff>
--- a/topic_ontologies_glittr.xlsx
+++ b/topic_ontologies_glittr.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geertvangeest/Documents/repositories/glittr-ontologies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67E023B-F07B-264F-B0FE-E99C35348499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F677C84-AEEF-8D41-9887-F48686E21A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="28920" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="500" windowWidth="26760" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Blad1!$B$1:$G$1017</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$I$1018</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="248">
   <si>
     <t>Containerization</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Presenting data and/or analysis in format that can be comprehended by and reproduced for stakeholders; can include anything related to reporting, building dashboards, creating data products, or repository sharing for analysis code</t>
   </si>
   <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
     <t>Data visualization</t>
   </si>
   <si>
@@ -286,12 +283,6 @@
     <t>Version control</t>
   </si>
   <si>
-    <t>Neuroscience Information Framework (NIF) Standard Ontology</t>
-  </si>
-  <si>
-    <t>http://uri.neuinfo.org/nif/nifstd/birnlex_2246</t>
-  </si>
-  <si>
     <t>A resource that provides a system for the management of multiple revisions of the same unit of information. It is most commonly used in engineering and software development to manage ongoing development of digital documents like application source code, art resources such as blueprints or electronic models, and other projects that may be worked on by a team of people.</t>
   </si>
   <si>
@@ -665,6 +656,186 @@
   </si>
   <si>
     <t xml:space="preserve">Make is a build automation tool that builds executable programs and libraries from source code by reading files called makefiles which specify how to derive the target program. </t>
+  </si>
+  <si>
+    <t>term_code</t>
+  </si>
+  <si>
+    <t>term_set</t>
+  </si>
+  <si>
+    <t>https://bio.tools</t>
+  </si>
+  <si>
+    <t>nextflow</t>
+  </si>
+  <si>
+    <t>snakemake</t>
+  </si>
+  <si>
+    <t>http://bigdatau.org/dseo</t>
+  </si>
+  <si>
+    <t>high_performance_computing</t>
+  </si>
+  <si>
+    <t>cloud_computing</t>
+  </si>
+  <si>
+    <t>reproducibility</t>
+  </si>
+  <si>
+    <t>Data Visualisation</t>
+  </si>
+  <si>
+    <t>http://edamontology.org</t>
+  </si>
+  <si>
+    <t>topic_0092</t>
+  </si>
+  <si>
+    <t>Unix_Linux</t>
+  </si>
+  <si>
+    <t>MATLAB_Octave</t>
+  </si>
+  <si>
+    <t>C_C++</t>
+  </si>
+  <si>
+    <t>format_3857</t>
+  </si>
+  <si>
+    <t>topic_0769</t>
+  </si>
+  <si>
+    <t>operation_3443</t>
+  </si>
+  <si>
+    <t>topic_3071</t>
+  </si>
+  <si>
+    <t>topic_4012</t>
+  </si>
+  <si>
+    <t>format_3788</t>
+  </si>
+  <si>
+    <t>topic_3305</t>
+  </si>
+  <si>
+    <t>topic_3169</t>
+  </si>
+  <si>
+    <t>topic_0797</t>
+  </si>
+  <si>
+    <t>operation_3501</t>
+  </si>
+  <si>
+    <t>topic_3295</t>
+  </si>
+  <si>
+    <t>operation_0362</t>
+  </si>
+  <si>
+    <t>operation_0525</t>
+  </si>
+  <si>
+    <t>topic_0622</t>
+  </si>
+  <si>
+    <t>topic_3174</t>
+  </si>
+  <si>
+    <t>topic_3301</t>
+  </si>
+  <si>
+    <t>topic_4021</t>
+  </si>
+  <si>
+    <t>topic_3168</t>
+  </si>
+  <si>
+    <t>topic_3170</t>
+  </si>
+  <si>
+    <t>topic_4028</t>
+  </si>
+  <si>
+    <t>topic_3308</t>
+  </si>
+  <si>
+    <t>operation_3504</t>
+  </si>
+  <si>
+    <t>topic_3172</t>
+  </si>
+  <si>
+    <t>topic_0121</t>
+  </si>
+  <si>
+    <t>data_2600</t>
+  </si>
+  <si>
+    <t>topic_3474</t>
+  </si>
+  <si>
+    <t>topic_2269</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/</t>
+  </si>
+  <si>
+    <t>EFO_0007045</t>
+  </si>
+  <si>
+    <t>EFO_0008994</t>
+  </si>
+  <si>
+    <t>EFO_0009989</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fdt/fdt-o</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MESH</t>
+  </si>
+  <si>
+    <t>D000077488</t>
+  </si>
+  <si>
+    <t>Biomedical Informatics Research Network Project Lexicon</t>
+  </si>
+  <si>
+    <t>birnlex_2246</t>
+  </si>
+  <si>
+    <t>http://bioontology.org/projects/ontologies/birnlex</t>
+  </si>
+  <si>
+    <t>http://bioontology.org/projects/ontologies/birnlex#birnlex_2246</t>
+  </si>
+  <si>
+    <t>Shiny_(software)</t>
+  </si>
+  <si>
+    <t>Julia_(programming_language)</t>
+  </si>
+  <si>
+    <t>Make_(software)</t>
+  </si>
+  <si>
+    <t>Containerization_(computing)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/</t>
+  </si>
+  <si>
+    <t>Containerization (computing)</t>
+  </si>
+  <si>
+    <t>In software engineering, containerization is operating system-level virtualization or application-level virtualization over multiple network resources so that software applications can run in isolated user spaces called containers in any cloud or non-cloud environment, regardless of type or vendor.</t>
   </si>
 </sst>
 </file>
@@ -765,9 +936,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -854,6 +1025,16 @@
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -863,12 +1044,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FFA4C2F4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -883,8 +1070,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -901,22 +1088,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB4A7D6"/>
           <bgColor rgb="FFB4A7D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA4C2F4"/>
-          <bgColor rgb="FFA4C2F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1134,10 +1305,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1017"/>
+  <dimension ref="A1:I1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1146,1236 +1317,1552 @@
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="108.1640625" customWidth="1"/>
+    <col min="5" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="108.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" ref="E2:E33" si="0">IF(D2=B2,"TRUE", "FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>IF(D2=B2,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D3=B3,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>IF(D4=B4,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D5=B5,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D6=B6,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F6" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D7=B7,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>IF(D8=B8,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>23</v>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D9=B9,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>IF(D10=B10,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>IF(D11=B11,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
+        <f>IF(D12=B12,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="I12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D13=B13,"TRUE", "FALSE")</f>
         <v>FALSE</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F13" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D14=B14,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F14" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
+        <v>74</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
+      <c r="D15" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D15=B15,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F15" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
+        <v>74</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D16=B16,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F16" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>12</v>
+        <v>90</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E17" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D17=B17,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F17" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>12</v>
+        <v>93</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="E18" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D18=B18,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
+      <c r="F18" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D19=B19,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="str">
+        <f>IF(D20=B20,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="3" t="str">
+        <f>IF(D21=B21,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="3" t="str">
+        <f>IF(D22=B22,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="3" t="str">
+        <f>IF(D23=B23,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="3" t="str">
+        <f>IF(D24=B24,"TRUE", "FALSE")</f>
         <v>FALSE</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="F24" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="3" t="str">
+        <f>IF(D25=B25,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="F25" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="3" t="str">
+        <f>IF(D26=B26,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="E25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F26" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
+        <v>74</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D27=B27,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F27" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D28=B28,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="3" t="str">
+        <f>IF(D29=B29,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="B30" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="3" t="str">
+        <f>IF(D30=B30,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F30" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D31" t="s">
-        <v>75</v>
+      <c r="D31" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(D31=B31,"TRUE", "FALSE")</f>
         <v>FALSE</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G31" t="s">
+      <c r="D32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="3" t="str">
+        <f>IF(D32=B32,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="3" t="str">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f>IF(D33=B33,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="F33" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="3" t="str">
+        <f>IF(D34=B34,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f>IF(D35=B35,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f>IF(D36=B36,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="3" t="str">
-        <f t="shared" ref="E34:E55" si="1">IF(D34=B34,"TRUE", "FALSE")</f>
-        <v>TRUE</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F36" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D37=B37,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F37" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D38=B38,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F38" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D39=B39,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F39" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D40=B40,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="6" t="s">
-        <v>77</v>
+      <c r="F40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>4</v>
+        <v>58</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D41=B41,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F41" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D42=B42,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
+      <c r="F42" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
-        <v>118</v>
+        <f>IF(D43=B43,"TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D44=B44,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F44" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" t="s">
-        <v>122</v>
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D45" t="s">
-        <v>121</v>
+      <c r="D45" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="E45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D45=B45,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f>IF(D46=B46,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F45" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" t="s">
-        <v>125</v>
-      </c>
-      <c r="E46" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="F46" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f>IF(D47=B47,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" s="3" t="str">
+        <f>IF(D48=B48,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f>IF(D49=B49,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G49" t="s">
+        <v>245</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f>IF(D50=B50,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G50" t="s">
+        <v>245</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="3" t="str">
+        <f>IF(D51=B51,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="3" t="str">
+        <f>IF(D52=B52,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="3" t="str">
+        <f>IF(D53=B53,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F46" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G48" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="F53" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>4</v>
@@ -2384,65 +2871,77 @@
         <v>146</v>
       </c>
       <c r="E54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(D54=B54,"TRUE", "FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="3" t="str">
+        <f>IF(D55=B55,"TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G54" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="6" t="s">
+      <c r="F55" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B55" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>149</v>
-      </c>
-      <c r="E55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="13"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="13"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="13"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="13"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="13"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="13"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="13"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="13"/>
     </row>
     <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5305,89 +5804,98 @@
       <c r="A1017" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G1017" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I1018" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1018">
+      <sortCondition ref="A1:A1018"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="A2:A210">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Statistics and machine learning">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Omics analysis">
+      <formula>NOT(ISERROR(SEARCH(("Omics analysis"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Computational methods and pipelines">
+      <formula>NOT(ISERROR(SEARCH(("Computational methods and pipelines"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Statistics and machine learning">
       <formula>NOT(ISERROR(SEARCH(("Statistics and machine learning"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Scripting and languages">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Others">
+      <formula>NOT(ISERROR(SEARCH(("Others"),(A2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Scripting and languages">
       <formula>NOT(ISERROR(SEARCH(("Scripting and languages"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Omics analysis">
-      <formula>NOT(ISERROR(SEARCH(("Omics analysis"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Computational methods and pipelines">
-      <formula>NOT(ISERROR(SEARCH(("Computational methods and pipelines"),(A2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Reproducibility and data management">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Reproducibility and data management">
       <formula>NOT(ISERROR(SEARCH(("Reproducibility and data management"),(A2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Others">
-      <formula>NOT(ISERROR(SEARCH(("Others"),(A2))))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 E2:G3 E4:F7 E9:F44 E53:G55 E51:F52 E45:G47 E49:G50 E48">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"TRUE"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E55">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FALSE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" location="Docker" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" location="Galaxy" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" location="high_performance_computing" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F8" r:id="rId6" location="Singularity" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F12" r:id="rId9" location="cloud_computing" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F16" r:id="rId12" location="reproducibility" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F17" r:id="rId13" location="data_visualization" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F18" r:id="rId14" location="Python" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F20" r:id="rId15" location="R" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F23" r:id="rId16" location="Unix_Linux" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F24" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F27" r:id="rId18" location="MATLAB_Octave" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F31" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F32" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F33" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F34" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F35" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F36" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F37" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="F38" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="F39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F40" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F41" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F44" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F45" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F46" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F47" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="F48" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F52" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="F53" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F54" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="F55" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="F29" r:id="rId42" location="Java" xr:uid="{3A663C11-DD57-8645-8EA4-87B1D3250EC5}"/>
-    <hyperlink ref="F30" r:id="rId43" location="C_C++" xr:uid="{C3B74948-F199-1447-B670-8BC72A89A5F8}"/>
-    <hyperlink ref="F7" r:id="rId44" xr:uid="{88DBBF94-CB57-854D-88FD-606D4268F8B7}"/>
-    <hyperlink ref="F9" r:id="rId45" xr:uid="{7D66D706-D109-6644-88B5-9B377B0A29ED}"/>
-    <hyperlink ref="F25" r:id="rId46" xr:uid="{702E6F8C-ECBA-AA45-BE7A-31BBABFD938B}"/>
-    <hyperlink ref="F26" r:id="rId47" xr:uid="{B464ED92-6ECB-FA47-B395-204A441448BD}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{A0059E1D-2F4F-F94D-A5C9-290682EE3BF6}"/>
-    <hyperlink ref="F50" r:id="rId49" xr:uid="{2A9A0FA4-3276-CA43-BC5E-8130D6536487}"/>
-    <hyperlink ref="F51" r:id="rId50" xr:uid="{E0B47E6A-ED88-8441-8475-761ED87B3B20}"/>
-    <hyperlink ref="F22" r:id="rId51" xr:uid="{C3FF2065-443C-594B-A3F7-7A818E41D753}"/>
+    <hyperlink ref="H50" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H10" r:id="rId3" location="Docker" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H4" r:id="rId4" location="Galaxy" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H5" r:id="rId5" location="high_performance_computing" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H11" r:id="rId6" location="Singularity" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H6" r:id="rId9" location="cloud_computing" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H37" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H38" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H36" r:id="rId12" location="reproducibility" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H39" r:id="rId13" location="Python" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H40" r:id="rId14" location="R" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H41" r:id="rId15" location="Unix_Linux" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H42" r:id="rId16" location="MATLAB_Octave" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H46" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H13" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H14" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H16" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H18" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H20" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H21" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H22" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H25" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H33" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H27" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H28" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H34" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H55" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H53" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H54" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H43" r:id="rId40" location="Java" xr:uid="{3A663C11-DD57-8645-8EA4-87B1D3250EC5}"/>
+    <hyperlink ref="H44" r:id="rId41" location="C_C++" xr:uid="{C3B74948-F199-1447-B670-8BC72A89A5F8}"/>
+    <hyperlink ref="H2" r:id="rId42" xr:uid="{88DBBF94-CB57-854D-88FD-606D4268F8B7}"/>
+    <hyperlink ref="H3" r:id="rId43" xr:uid="{7D66D706-D109-6644-88B5-9B377B0A29ED}"/>
+    <hyperlink ref="H48" r:id="rId44" xr:uid="{702E6F8C-ECBA-AA45-BE7A-31BBABFD938B}"/>
+    <hyperlink ref="H49" r:id="rId45" xr:uid="{B464ED92-6ECB-FA47-B395-204A441448BD}"/>
+    <hyperlink ref="H29" r:id="rId46" xr:uid="{A0059E1D-2F4F-F94D-A5C9-290682EE3BF6}"/>
+    <hyperlink ref="H30" r:id="rId47" xr:uid="{2A9A0FA4-3276-CA43-BC5E-8130D6536487}"/>
+    <hyperlink ref="H31" r:id="rId48" xr:uid="{E0B47E6A-ED88-8441-8475-761ED87B3B20}"/>
+    <hyperlink ref="H47" r:id="rId49" xr:uid="{C3FF2065-443C-594B-A3F7-7A818E41D753}"/>
+    <hyperlink ref="G3" r:id="rId50" xr:uid="{15299088-2FB7-6F42-B25F-F9152D395130}"/>
+    <hyperlink ref="H45" r:id="rId51" location="data_visualization" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G45" r:id="rId52" xr:uid="{C4CBEE97-9D4B-EC4F-8B0B-7ED55B5F4AFC}"/>
+    <hyperlink ref="G15:G41" r:id="rId53" display="http://edamontology.org" xr:uid="{EBDD7A00-AFA3-C649-BEC4-87B510883EF0}"/>
+    <hyperlink ref="G55" r:id="rId54" xr:uid="{A800D5BC-8FAE-5A48-9D94-5631162D32D4}"/>
+    <hyperlink ref="C12" r:id="rId55" display="https://bioportal.bioontology.org/ontologies/BIRNLEX" xr:uid="{A00ED0B1-1655-3D46-930D-EE5547C28515}"/>
+    <hyperlink ref="G12" r:id="rId56" xr:uid="{3E958A3C-528E-8F42-9910-E3DAD9E143F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId52"/>
+  <legacyDrawing r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>